<commit_message>
Modulaire and Questions extract ok
</commit_message>
<xml_diff>
--- a/tmplt.xlsx
+++ b/tmplt.xlsx
@@ -539,7 +539,17 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q1 : ANALYSE DES RISQUES
+Quels sont les risques engendrés par cette situation
+Evaluer ces risques
+Identifier ceux qui sont critiques – et pourquoi (vous pouvez vous servir de la matrice de criticité des risques)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr"/>
       <c r="P2" t="n">
@@ -571,7 +581,17 @@
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q2 : DECLENCHEMENT DE L’AUDIT
+Qui mandate l’audit
+Qui va réaliser l’audit (vous pouvez choisir interne ou externe)
+Sur quels critères l’auditeur est choisi ?
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N3" t="inlineStr"/>
       <c r="O3" t="inlineStr"/>
       <c r="P3" t="n">
@@ -603,7 +623,17 @@
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q3 : PLANIFICATION DE L’AUDIT
+Quelles sont les étapes de l’audit
+Etablir le planning de l’audit (en tenant compte des dates prévues)
+Identifier les acteurs de l’audit et leurs responsabilités (utiliser la matrice RACI)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr"/>
       <c r="P4" t="n">
@@ -635,7 +665,15 @@
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q4 : ANALYSE DOCUMENTAIRE
+Quels sont les documents qui pourraient vous aider à préparer cet audit ? (Soyez précis, vous pouvez identifier des documents que DISTRELEC pourrait avoir)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="inlineStr"/>
       <c r="P5" t="n">
@@ -667,7 +705,16 @@
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr"/>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q5 : REALISATION DE L’AUDIT
+Identifier 3 personnes (fonctions) à auditer
+Elaborer le guide d’entretien pour l’un des audités (préciser lequel)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N6" t="inlineStr"/>
       <c r="O6" t="inlineStr"/>
       <c r="P6" t="n">
@@ -699,7 +746,18 @@
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr"/>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q6 : CONCLUSIONS DE L’AUDIT
+Rédiger votre conclusion (à imaginer) présentant : 
+☞ 1 point fort
+☞ 2 points sensibles
+☞ 2 écarts
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr"/>
       <c r="P7" t="n">
@@ -731,7 +789,15 @@
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q7 : RECHERCHE DES CAUSES
+Pour chaque écart relevé identifier faite une analyse des causes (en utilisant le diagramme 5M)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="inlineStr"/>
       <c r="P8" t="n">
@@ -763,7 +829,17 @@
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q8 : SOLUTIONS
+Trouver 2 solutions pour chaque écart : 
+☞ Préciser à quelles causes elles correspondent
+☞ Décrire les solutions
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr"/>
       <c r="P9" t="n">
@@ -795,7 +871,17 @@
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q1 : ANALYSE DES RISQUES
+Quels sont les risques engendrés par cette situation
+Evaluer ces risques
+Identifier ceux qui sont critiques – et pourquoi (vous pouvez vous servir de la matrice de criticité des risques)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr"/>
       <c r="P10" t="n">
@@ -827,7 +913,17 @@
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q2 : DECLENCHEMENT DE L’AUDIT
+Qui mandate l’audit
+Qui va réaliser l’audit (vous pouvez choisir interne ou externe)
+Sur quels critères l’auditeur est choisi ?
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="inlineStr"/>
       <c r="P11" t="n">
@@ -859,7 +955,17 @@
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr"/>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q3 : PLANIFICATION DE L’AUDIT
+Quelles sont les étapes de l’audit
+Etablir le planning de l’audit (en tenant compte des dates prévues)
+Identifier les acteurs de l’audit et leurs responsabilités (utiliser la matrice RACI)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N12" t="inlineStr"/>
       <c r="O12" t="inlineStr"/>
       <c r="P12" t="n">
@@ -891,7 +997,15 @@
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr"/>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q4 : ANALYSE DOCUMENTAIRE
+Quels sont les documents qui pourraient vous aider à préparer cet audit ? (Soyez précis, vous pouvez identifier des documents que DISTRELEC pourrait avoir)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="inlineStr"/>
       <c r="P13" t="n">
@@ -923,7 +1037,16 @@
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr"/>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q5 : REALISATION DE L’AUDIT
+Identifier 3 personnes (fonctions) à auditer
+Elaborer le guide d’entretien pour l’un des audités (préciser lequel)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="inlineStr"/>
       <c r="P14" t="n">
@@ -955,7 +1078,18 @@
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr"/>
-      <c r="M15" t="inlineStr"/>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q6 : CONCLUSIONS DE L’AUDIT
+Rédiger votre conclusion (à imaginer) présentant : 
+☞ 1 point fort
+☞ 2 points sensibles
+☞ 2 écarts
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N15" t="inlineStr"/>
       <c r="O15" t="inlineStr"/>
       <c r="P15" t="n">
@@ -987,7 +1121,15 @@
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr"/>
-      <c r="M16" t="inlineStr"/>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q7 : RECHERCHE DES CAUSES
+Pour chaque écart relevé identifier faite une analyse des causes (en utilisant le diagramme 5M)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N16" t="inlineStr"/>
       <c r="O16" t="inlineStr"/>
       <c r="P16" t="n">
@@ -1019,7 +1161,17 @@
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="inlineStr"/>
       <c r="L17" t="inlineStr"/>
-      <c r="M17" t="inlineStr"/>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q8 : SOLUTIONS
+Trouver 2 solutions pour chaque écart : 
+☞ Préciser à quelles causes elles correspondent
+☞ Décrire les solutions
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N17" t="inlineStr"/>
       <c r="O17" t="inlineStr"/>
       <c r="P17" t="n">
@@ -1051,7 +1203,17 @@
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr"/>
       <c r="L18" t="inlineStr"/>
-      <c r="M18" t="inlineStr"/>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q1 : ANALYSE DES RISQUES
+Quels sont les risques engendrés par cette situation
+Evaluer ces risques
+Identifier ceux qui sont critiques – et pourquoi (vous pouvez vous servir de la matrice de criticité des risques)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N18" t="inlineStr"/>
       <c r="O18" t="inlineStr"/>
       <c r="P18" t="n">
@@ -1083,7 +1245,17 @@
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr"/>
-      <c r="M19" t="inlineStr"/>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q2 : DECLENCHEMENT DE L’AUDIT
+Qui mandate l’audit
+Qui va réaliser l’audit (vous pouvez choisir interne ou externe)
+Sur quels critères l’auditeur est choisi ?
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N19" t="inlineStr"/>
       <c r="O19" t="inlineStr"/>
       <c r="P19" t="n">
@@ -1115,7 +1287,17 @@
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr"/>
-      <c r="M20" t="inlineStr"/>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q3 : PLANIFICATION DE L’AUDIT
+Quelles sont les étapes de l’audit
+Etablir le planning de l’audit (en tenant compte des dates prévues)
+Identifier les acteurs de l’audit et leurs responsabilités (utiliser la matrice RACI)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N20" t="inlineStr"/>
       <c r="O20" t="inlineStr"/>
       <c r="P20" t="n">
@@ -1147,7 +1329,15 @@
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr"/>
-      <c r="M21" t="inlineStr"/>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q4 : ANALYSE DOCUMENTAIRE
+Quels sont les documents qui pourraient vous aider à préparer cet audit ? (Soyez précis, vous pouvez identifier des documents que DISTRELEC pourrait avoir)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N21" t="inlineStr"/>
       <c r="O21" t="inlineStr"/>
       <c r="P21" t="n">
@@ -1179,7 +1369,16 @@
       <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr"/>
-      <c r="M22" t="inlineStr"/>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q5 : REALISATION DE L’AUDIT
+Identifier 3 personnes (fonctions) à auditer
+Elaborer le guide d’entretien pour l’un des audités (préciser lequel)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N22" t="inlineStr"/>
       <c r="O22" t="inlineStr"/>
       <c r="P22" t="n">
@@ -1211,7 +1410,18 @@
       <c r="J23" t="inlineStr"/>
       <c r="K23" t="inlineStr"/>
       <c r="L23" t="inlineStr"/>
-      <c r="M23" t="inlineStr"/>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q6 : CONCLUSIONS DE L’AUDIT
+Rédiger votre conclusion (à imaginer) présentant : 
+☞ 1 point fort
+☞ 2 points sensibles
+☞ 2 écarts
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N23" t="inlineStr"/>
       <c r="O23" t="inlineStr"/>
       <c r="P23" t="n">
@@ -1243,7 +1453,15 @@
       <c r="J24" t="inlineStr"/>
       <c r="K24" t="inlineStr"/>
       <c r="L24" t="inlineStr"/>
-      <c r="M24" t="inlineStr"/>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q7 : RECHERCHE DES CAUSES
+Pour chaque écart relevé identifier faite une analyse des causes (en utilisant le diagramme 5M)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N24" t="inlineStr"/>
       <c r="O24" t="inlineStr"/>
       <c r="P24" t="n">
@@ -1275,7 +1493,17 @@
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr"/>
-      <c r="M25" t="inlineStr"/>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q8 : SOLUTIONS
+Trouver 2 solutions pour chaque écart : 
+☞ Préciser à quelles causes elles correspondent
+☞ Décrire les solutions
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N25" t="inlineStr"/>
       <c r="O25" t="inlineStr"/>
       <c r="P25" t="n">
@@ -1307,7 +1535,17 @@
       <c r="J26" t="inlineStr"/>
       <c r="K26" t="inlineStr"/>
       <c r="L26" t="inlineStr"/>
-      <c r="M26" t="inlineStr"/>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q1 : ANALYSE DES RISQUES
+Quels sont les risques engendrés par cette situation
+Evaluer ces risques
+Identifier ceux qui sont critiques – et pourquoi (vous pouvez vous servir de la matrice de criticité des risques)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N26" t="inlineStr"/>
       <c r="O26" t="inlineStr"/>
       <c r="P26" t="n">
@@ -1339,7 +1577,17 @@
       <c r="J27" t="inlineStr"/>
       <c r="K27" t="inlineStr"/>
       <c r="L27" t="inlineStr"/>
-      <c r="M27" t="inlineStr"/>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q2 : DECLENCHEMENT DE L’AUDIT
+Qui mandate l’audit
+Qui va réaliser l’audit (vous pouvez choisir interne ou externe)
+Sur quels critères l’auditeur est choisi ?
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N27" t="inlineStr"/>
       <c r="O27" t="inlineStr"/>
       <c r="P27" t="n">
@@ -1371,7 +1619,17 @@
       <c r="J28" t="inlineStr"/>
       <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr"/>
-      <c r="M28" t="inlineStr"/>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q3 : PLANIFICATION DE L’AUDIT
+Quelles sont les étapes de l’audit
+Etablir le planning de l’audit (en tenant compte des dates prévues)
+Identifier les acteurs de l’audit et leurs responsabilités (utiliser la matrice RACI)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N28" t="inlineStr"/>
       <c r="O28" t="inlineStr"/>
       <c r="P28" t="n">
@@ -1403,7 +1661,15 @@
       <c r="J29" t="inlineStr"/>
       <c r="K29" t="inlineStr"/>
       <c r="L29" t="inlineStr"/>
-      <c r="M29" t="inlineStr"/>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q4 : ANALYSE DOCUMENTAIRE
+Quels sont les documents qui pourraient vous aider à préparer cet audit ? (Soyez précis, vous pouvez identifier des documents que DISTRELEC pourrait avoir)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N29" t="inlineStr"/>
       <c r="O29" t="inlineStr"/>
       <c r="P29" t="n">
@@ -1435,7 +1701,16 @@
       <c r="J30" t="inlineStr"/>
       <c r="K30" t="inlineStr"/>
       <c r="L30" t="inlineStr"/>
-      <c r="M30" t="inlineStr"/>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q5 : REALISATION DE L’AUDIT
+Identifier 3 personnes (fonctions) à auditer
+Elaborer le guide d’entretien pour l’un des audités (préciser lequel)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N30" t="inlineStr"/>
       <c r="O30" t="inlineStr"/>
       <c r="P30" t="n">
@@ -1467,7 +1742,18 @@
       <c r="J31" t="inlineStr"/>
       <c r="K31" t="inlineStr"/>
       <c r="L31" t="inlineStr"/>
-      <c r="M31" t="inlineStr"/>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q6 : CONCLUSIONS DE L’AUDIT
+Rédiger votre conclusion (à imaginer) présentant : 
+☞ 1 point fort
+☞ 2 points sensibles
+☞ 2 écarts
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N31" t="inlineStr"/>
       <c r="O31" t="inlineStr"/>
       <c r="P31" t="n">
@@ -1499,7 +1785,15 @@
       <c r="J32" t="inlineStr"/>
       <c r="K32" t="inlineStr"/>
       <c r="L32" t="inlineStr"/>
-      <c r="M32" t="inlineStr"/>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q7 : RECHERCHE DES CAUSES
+Pour chaque écart relevé identifier faite une analyse des causes (en utilisant le diagramme 5M)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N32" t="inlineStr"/>
       <c r="O32" t="inlineStr"/>
       <c r="P32" t="n">
@@ -1531,7 +1825,17 @@
       <c r="J33" t="inlineStr"/>
       <c r="K33" t="inlineStr"/>
       <c r="L33" t="inlineStr"/>
-      <c r="M33" t="inlineStr"/>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q8 : SOLUTIONS
+Trouver 2 solutions pour chaque écart : 
+☞ Préciser à quelles causes elles correspondent
+☞ Décrire les solutions
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N33" t="inlineStr"/>
       <c r="O33" t="inlineStr"/>
       <c r="P33" t="n">
@@ -1563,7 +1867,17 @@
       <c r="J34" t="inlineStr"/>
       <c r="K34" t="inlineStr"/>
       <c r="L34" t="inlineStr"/>
-      <c r="M34" t="inlineStr"/>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q1 : ANALYSE DES RISQUES
+Quels sont les risques engendrés par cette situation
+Evaluer ces risques
+Identifier ceux qui sont critiques – et pourquoi (vous pouvez vous servir de la matrice de criticité des risques)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N34" t="inlineStr"/>
       <c r="O34" t="inlineStr"/>
       <c r="P34" t="n">
@@ -1595,7 +1909,17 @@
       <c r="J35" t="inlineStr"/>
       <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr"/>
-      <c r="M35" t="inlineStr"/>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q2 : DECLENCHEMENT DE L’AUDIT
+Qui mandate l’audit
+Qui va réaliser l’audit (vous pouvez choisir interne ou externe)
+Sur quels critères l’auditeur est choisi ?
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N35" t="inlineStr"/>
       <c r="O35" t="inlineStr"/>
       <c r="P35" t="n">
@@ -1627,7 +1951,17 @@
       <c r="J36" t="inlineStr"/>
       <c r="K36" t="inlineStr"/>
       <c r="L36" t="inlineStr"/>
-      <c r="M36" t="inlineStr"/>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q3 : PLANIFICATION DE L’AUDIT
+Quelles sont les étapes de l’audit
+Etablir le planning de l’audit (en tenant compte des dates prévues)
+Identifier les acteurs de l’audit et leurs responsabilités (utiliser la matrice RACI)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N36" t="inlineStr"/>
       <c r="O36" t="inlineStr"/>
       <c r="P36" t="n">
@@ -1659,7 +1993,15 @@
       <c r="J37" t="inlineStr"/>
       <c r="K37" t="inlineStr"/>
       <c r="L37" t="inlineStr"/>
-      <c r="M37" t="inlineStr"/>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q4 : ANALYSE DOCUMENTAIRE
+Quels sont les documents qui pourraient vous aider à préparer cet audit ? (Soyez précis, vous pouvez identifier des documents que DISTRELEC pourrait avoir)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N37" t="inlineStr"/>
       <c r="O37" t="inlineStr"/>
       <c r="P37" t="n">
@@ -1691,7 +2033,16 @@
       <c r="J38" t="inlineStr"/>
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr"/>
-      <c r="M38" t="inlineStr"/>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q5 : REALISATION DE L’AUDIT
+Identifier 3 personnes (fonctions) à auditer
+Elaborer le guide d’entretien pour l’un des audités (préciser lequel)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N38" t="inlineStr"/>
       <c r="O38" t="inlineStr"/>
       <c r="P38" t="n">
@@ -1723,7 +2074,18 @@
       <c r="J39" t="inlineStr"/>
       <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr"/>
-      <c r="M39" t="inlineStr"/>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q6 : CONCLUSIONS DE L’AUDIT
+Rédiger votre conclusion (à imaginer) présentant : 
+☞ 1 point fort
+☞ 2 points sensibles
+☞ 2 écarts
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N39" t="inlineStr"/>
       <c r="O39" t="inlineStr"/>
       <c r="P39" t="n">
@@ -1755,7 +2117,15 @@
       <c r="J40" t="inlineStr"/>
       <c r="K40" t="inlineStr"/>
       <c r="L40" t="inlineStr"/>
-      <c r="M40" t="inlineStr"/>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q7 : RECHERCHE DES CAUSES
+Pour chaque écart relevé identifier faite une analyse des causes (en utilisant le diagramme 5M)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N40" t="inlineStr"/>
       <c r="O40" t="inlineStr"/>
       <c r="P40" t="n">
@@ -1787,7 +2157,17 @@
       <c r="J41" t="inlineStr"/>
       <c r="K41" t="inlineStr"/>
       <c r="L41" t="inlineStr"/>
-      <c r="M41" t="inlineStr"/>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q8 : SOLUTIONS
+Trouver 2 solutions pour chaque écart : 
+☞ Préciser à quelles causes elles correspondent
+☞ Décrire les solutions
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N41" t="inlineStr"/>
       <c r="O41" t="inlineStr"/>
       <c r="P41" t="n">
@@ -1819,7 +2199,17 @@
       <c r="J42" t="inlineStr"/>
       <c r="K42" t="inlineStr"/>
       <c r="L42" t="inlineStr"/>
-      <c r="M42" t="inlineStr"/>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q1 : ANALYSE DES RISQUES
+Quels sont les risques engendrés par cette situation
+Evaluer ces risques
+Identifier ceux qui sont critiques – et pourquoi (vous pouvez vous servir de la matrice de criticité des risques)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N42" t="inlineStr"/>
       <c r="O42" t="inlineStr"/>
       <c r="P42" t="n">
@@ -1851,7 +2241,17 @@
       <c r="J43" t="inlineStr"/>
       <c r="K43" t="inlineStr"/>
       <c r="L43" t="inlineStr"/>
-      <c r="M43" t="inlineStr"/>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q2 : DECLENCHEMENT DE L’AUDIT
+Qui mandate l’audit
+Qui va réaliser l’audit (vous pouvez choisir interne ou externe)
+Sur quels critères l’auditeur est choisi ?
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N43" t="inlineStr"/>
       <c r="O43" t="inlineStr"/>
       <c r="P43" t="n">
@@ -1883,7 +2283,17 @@
       <c r="J44" t="inlineStr"/>
       <c r="K44" t="inlineStr"/>
       <c r="L44" t="inlineStr"/>
-      <c r="M44" t="inlineStr"/>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q3 : PLANIFICATION DE L’AUDIT
+Quelles sont les étapes de l’audit
+Etablir le planning de l’audit (en tenant compte des dates prévues)
+Identifier les acteurs de l’audit et leurs responsabilités (utiliser la matrice RACI)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N44" t="inlineStr"/>
       <c r="O44" t="inlineStr"/>
       <c r="P44" t="n">
@@ -1915,7 +2325,15 @@
       <c r="J45" t="inlineStr"/>
       <c r="K45" t="inlineStr"/>
       <c r="L45" t="inlineStr"/>
-      <c r="M45" t="inlineStr"/>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q4 : ANALYSE DOCUMENTAIRE
+Quels sont les documents qui pourraient vous aider à préparer cet audit ? (Soyez précis, vous pouvez identifier des documents que DISTRELEC pourrait avoir)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N45" t="inlineStr"/>
       <c r="O45" t="inlineStr"/>
       <c r="P45" t="n">
@@ -1947,7 +2365,16 @@
       <c r="J46" t="inlineStr"/>
       <c r="K46" t="inlineStr"/>
       <c r="L46" t="inlineStr"/>
-      <c r="M46" t="inlineStr"/>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q5 : REALISATION DE L’AUDIT
+Identifier 3 personnes (fonctions) à auditer
+Elaborer le guide d’entretien pour l’un des audités (préciser lequel)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N46" t="inlineStr"/>
       <c r="O46" t="inlineStr"/>
       <c r="P46" t="n">
@@ -1979,7 +2406,18 @@
       <c r="J47" t="inlineStr"/>
       <c r="K47" t="inlineStr"/>
       <c r="L47" t="inlineStr"/>
-      <c r="M47" t="inlineStr"/>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q6 : CONCLUSIONS DE L’AUDIT
+Rédiger votre conclusion (à imaginer) présentant : 
+☞ 1 point fort
+☞ 2 points sensibles
+☞ 2 écarts
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N47" t="inlineStr"/>
       <c r="O47" t="inlineStr"/>
       <c r="P47" t="n">
@@ -2011,7 +2449,15 @@
       <c r="J48" t="inlineStr"/>
       <c r="K48" t="inlineStr"/>
       <c r="L48" t="inlineStr"/>
-      <c r="M48" t="inlineStr"/>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q7 : RECHERCHE DES CAUSES
+Pour chaque écart relevé identifier faite une analyse des causes (en utilisant le diagramme 5M)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N48" t="inlineStr"/>
       <c r="O48" t="inlineStr"/>
       <c r="P48" t="n">
@@ -2043,7 +2489,17 @@
       <c r="J49" t="inlineStr"/>
       <c r="K49" t="inlineStr"/>
       <c r="L49" t="inlineStr"/>
-      <c r="M49" t="inlineStr"/>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q8 : SOLUTIONS
+Trouver 2 solutions pour chaque écart : 
+☞ Préciser à quelles causes elles correspondent
+☞ Décrire les solutions
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N49" t="inlineStr"/>
       <c r="O49" t="inlineStr"/>
       <c r="P49" t="n">
@@ -2075,7 +2531,17 @@
       <c r="J50" t="inlineStr"/>
       <c r="K50" t="inlineStr"/>
       <c r="L50" t="inlineStr"/>
-      <c r="M50" t="inlineStr"/>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q1 : ANALYSE DES RISQUES
+Quels sont les risques engendrés par cette situation
+Evaluer ces risques
+Identifier ceux qui sont critiques – et pourquoi (vous pouvez vous servir de la matrice de criticité des risques)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N50" t="inlineStr"/>
       <c r="O50" t="inlineStr"/>
       <c r="P50" t="n">
@@ -2107,7 +2573,17 @@
       <c r="J51" t="inlineStr"/>
       <c r="K51" t="inlineStr"/>
       <c r="L51" t="inlineStr"/>
-      <c r="M51" t="inlineStr"/>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q2 : DECLENCHEMENT DE L’AUDIT
+Qui mandate l’audit
+Qui va réaliser l’audit (vous pouvez choisir interne ou externe)
+Sur quels critères l’auditeur est choisi ?
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N51" t="inlineStr"/>
       <c r="O51" t="inlineStr"/>
       <c r="P51" t="n">
@@ -2139,7 +2615,17 @@
       <c r="J52" t="inlineStr"/>
       <c r="K52" t="inlineStr"/>
       <c r="L52" t="inlineStr"/>
-      <c r="M52" t="inlineStr"/>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q3 : PLANIFICATION DE L’AUDIT
+Quelles sont les étapes de l’audit
+Etablir le planning de l’audit (en tenant compte des dates prévues)
+Identifier les acteurs de l’audit et leurs responsabilités (utiliser la matrice RACI)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N52" t="inlineStr"/>
       <c r="O52" t="inlineStr"/>
       <c r="P52" t="n">
@@ -2171,7 +2657,15 @@
       <c r="J53" t="inlineStr"/>
       <c r="K53" t="inlineStr"/>
       <c r="L53" t="inlineStr"/>
-      <c r="M53" t="inlineStr"/>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q4 : ANALYSE DOCUMENTAIRE
+Quels sont les documents qui pourraient vous aider à préparer cet audit ? (Soyez précis, vous pouvez identifier des documents que DISTRELEC pourrait avoir)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N53" t="inlineStr"/>
       <c r="O53" t="inlineStr"/>
       <c r="P53" t="n">
@@ -2203,7 +2697,16 @@
       <c r="J54" t="inlineStr"/>
       <c r="K54" t="inlineStr"/>
       <c r="L54" t="inlineStr"/>
-      <c r="M54" t="inlineStr"/>
+      <c r="M54" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q5 : REALISATION DE L’AUDIT
+Identifier 3 personnes (fonctions) à auditer
+Elaborer le guide d’entretien pour l’un des audités (préciser lequel)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N54" t="inlineStr"/>
       <c r="O54" t="inlineStr"/>
       <c r="P54" t="n">
@@ -2235,7 +2738,18 @@
       <c r="J55" t="inlineStr"/>
       <c r="K55" t="inlineStr"/>
       <c r="L55" t="inlineStr"/>
-      <c r="M55" t="inlineStr"/>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q6 : CONCLUSIONS DE L’AUDIT
+Rédiger votre conclusion (à imaginer) présentant : 
+☞ 1 point fort
+☞ 2 points sensibles
+☞ 2 écarts
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N55" t="inlineStr"/>
       <c r="O55" t="inlineStr"/>
       <c r="P55" t="n">
@@ -2267,7 +2781,15 @@
       <c r="J56" t="inlineStr"/>
       <c r="K56" t="inlineStr"/>
       <c r="L56" t="inlineStr"/>
-      <c r="M56" t="inlineStr"/>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q7 : RECHERCHE DES CAUSES
+Pour chaque écart relevé identifier faite une analyse des causes (en utilisant le diagramme 5M)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N56" t="inlineStr"/>
       <c r="O56" t="inlineStr"/>
       <c r="P56" t="n">
@@ -2299,7 +2821,17 @@
       <c r="J57" t="inlineStr"/>
       <c r="K57" t="inlineStr"/>
       <c r="L57" t="inlineStr"/>
-      <c r="M57" t="inlineStr"/>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q8 : SOLUTIONS
+Trouver 2 solutions pour chaque écart : 
+☞ Préciser à quelles causes elles correspondent
+☞ Décrire les solutions
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N57" t="inlineStr"/>
       <c r="O57" t="inlineStr"/>
       <c r="P57" t="n">
@@ -2331,7 +2863,17 @@
       <c r="J58" t="inlineStr"/>
       <c r="K58" t="inlineStr"/>
       <c r="L58" t="inlineStr"/>
-      <c r="M58" t="inlineStr"/>
+      <c r="M58" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q1 : ANALYSE DES RISQUES
+Quels sont les risques engendrés par cette situation
+Evaluer ces risques
+Identifier ceux qui sont critiques – et pourquoi (vous pouvez vous servir de la matrice de criticité des risques)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N58" t="inlineStr"/>
       <c r="O58" t="inlineStr"/>
       <c r="P58" t="n">
@@ -2363,7 +2905,17 @@
       <c r="J59" t="inlineStr"/>
       <c r="K59" t="inlineStr"/>
       <c r="L59" t="inlineStr"/>
-      <c r="M59" t="inlineStr"/>
+      <c r="M59" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q2 : DECLENCHEMENT DE L’AUDIT
+Qui mandate l’audit
+Qui va réaliser l’audit (vous pouvez choisir interne ou externe)
+Sur quels critères l’auditeur est choisi ?
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N59" t="inlineStr"/>
       <c r="O59" t="inlineStr"/>
       <c r="P59" t="n">
@@ -2395,7 +2947,17 @@
       <c r="J60" t="inlineStr"/>
       <c r="K60" t="inlineStr"/>
       <c r="L60" t="inlineStr"/>
-      <c r="M60" t="inlineStr"/>
+      <c r="M60" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q3 : PLANIFICATION DE L’AUDIT
+Quelles sont les étapes de l’audit
+Etablir le planning de l’audit (en tenant compte des dates prévues)
+Identifier les acteurs de l’audit et leurs responsabilités (utiliser la matrice RACI)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N60" t="inlineStr"/>
       <c r="O60" t="inlineStr"/>
       <c r="P60" t="n">
@@ -2427,7 +2989,15 @@
       <c r="J61" t="inlineStr"/>
       <c r="K61" t="inlineStr"/>
       <c r="L61" t="inlineStr"/>
-      <c r="M61" t="inlineStr"/>
+      <c r="M61" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q4 : ANALYSE DOCUMENTAIRE
+Quels sont les documents qui pourraient vous aider à préparer cet audit ? (Soyez précis, vous pouvez identifier des documents que DISTRELEC pourrait avoir)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N61" t="inlineStr"/>
       <c r="O61" t="inlineStr"/>
       <c r="P61" t="n">
@@ -2459,7 +3029,16 @@
       <c r="J62" t="inlineStr"/>
       <c r="K62" t="inlineStr"/>
       <c r="L62" t="inlineStr"/>
-      <c r="M62" t="inlineStr"/>
+      <c r="M62" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q5 : REALISATION DE L’AUDIT
+Identifier 3 personnes (fonctions) à auditer
+Elaborer le guide d’entretien pour l’un des audités (préciser lequel)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N62" t="inlineStr"/>
       <c r="O62" t="inlineStr"/>
       <c r="P62" t="n">
@@ -2491,7 +3070,18 @@
       <c r="J63" t="inlineStr"/>
       <c r="K63" t="inlineStr"/>
       <c r="L63" t="inlineStr"/>
-      <c r="M63" t="inlineStr"/>
+      <c r="M63" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q6 : CONCLUSIONS DE L’AUDIT
+Rédiger votre conclusion (à imaginer) présentant : 
+☞ 1 point fort
+☞ 2 points sensibles
+☞ 2 écarts
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N63" t="inlineStr"/>
       <c r="O63" t="inlineStr"/>
       <c r="P63" t="n">
@@ -2523,7 +3113,15 @@
       <c r="J64" t="inlineStr"/>
       <c r="K64" t="inlineStr"/>
       <c r="L64" t="inlineStr"/>
-      <c r="M64" t="inlineStr"/>
+      <c r="M64" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q7 : RECHERCHE DES CAUSES
+Pour chaque écart relevé identifier faite une analyse des causes (en utilisant le diagramme 5M)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N64" t="inlineStr"/>
       <c r="O64" t="inlineStr"/>
       <c r="P64" t="n">
@@ -2555,7 +3153,17 @@
       <c r="J65" t="inlineStr"/>
       <c r="K65" t="inlineStr"/>
       <c r="L65" t="inlineStr"/>
-      <c r="M65" t="inlineStr"/>
+      <c r="M65" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q8 : SOLUTIONS
+Trouver 2 solutions pour chaque écart : 
+☞ Préciser à quelles causes elles correspondent
+☞ Décrire les solutions
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N65" t="inlineStr"/>
       <c r="O65" t="inlineStr"/>
       <c r="P65" t="n">
@@ -2587,7 +3195,17 @@
       <c r="J66" t="inlineStr"/>
       <c r="K66" t="inlineStr"/>
       <c r="L66" t="inlineStr"/>
-      <c r="M66" t="inlineStr"/>
+      <c r="M66" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q1 : ANALYSE DES RISQUES
+Quels sont les risques engendrés par cette situation
+Evaluer ces risques
+Identifier ceux qui sont critiques – et pourquoi (vous pouvez vous servir de la matrice de criticité des risques)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N66" t="inlineStr"/>
       <c r="O66" t="inlineStr"/>
       <c r="P66" t="n">
@@ -2619,7 +3237,17 @@
       <c r="J67" t="inlineStr"/>
       <c r="K67" t="inlineStr"/>
       <c r="L67" t="inlineStr"/>
-      <c r="M67" t="inlineStr"/>
+      <c r="M67" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q2 : DECLENCHEMENT DE L’AUDIT
+Qui mandate l’audit
+Qui va réaliser l’audit (vous pouvez choisir interne ou externe)
+Sur quels critères l’auditeur est choisi ?
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N67" t="inlineStr"/>
       <c r="O67" t="inlineStr"/>
       <c r="P67" t="n">
@@ -2651,7 +3279,17 @@
       <c r="J68" t="inlineStr"/>
       <c r="K68" t="inlineStr"/>
       <c r="L68" t="inlineStr"/>
-      <c r="M68" t="inlineStr"/>
+      <c r="M68" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q3 : PLANIFICATION DE L’AUDIT
+Quelles sont les étapes de l’audit
+Etablir le planning de l’audit (en tenant compte des dates prévues)
+Identifier les acteurs de l’audit et leurs responsabilités (utiliser la matrice RACI)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N68" t="inlineStr"/>
       <c r="O68" t="inlineStr"/>
       <c r="P68" t="n">
@@ -2683,7 +3321,15 @@
       <c r="J69" t="inlineStr"/>
       <c r="K69" t="inlineStr"/>
       <c r="L69" t="inlineStr"/>
-      <c r="M69" t="inlineStr"/>
+      <c r="M69" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q4 : ANALYSE DOCUMENTAIRE
+Quels sont les documents qui pourraient vous aider à préparer cet audit ? (Soyez précis, vous pouvez identifier des documents que DISTRELEC pourrait avoir)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N69" t="inlineStr"/>
       <c r="O69" t="inlineStr"/>
       <c r="P69" t="n">
@@ -2715,7 +3361,16 @@
       <c r="J70" t="inlineStr"/>
       <c r="K70" t="inlineStr"/>
       <c r="L70" t="inlineStr"/>
-      <c r="M70" t="inlineStr"/>
+      <c r="M70" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q5 : REALISATION DE L’AUDIT
+Identifier 3 personnes (fonctions) à auditer
+Elaborer le guide d’entretien pour l’un des audités (préciser lequel)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N70" t="inlineStr"/>
       <c r="O70" t="inlineStr"/>
       <c r="P70" t="n">
@@ -2747,7 +3402,18 @@
       <c r="J71" t="inlineStr"/>
       <c r="K71" t="inlineStr"/>
       <c r="L71" t="inlineStr"/>
-      <c r="M71" t="inlineStr"/>
+      <c r="M71" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q6 : CONCLUSIONS DE L’AUDIT
+Rédiger votre conclusion (à imaginer) présentant : 
+☞ 1 point fort
+☞ 2 points sensibles
+☞ 2 écarts
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N71" t="inlineStr"/>
       <c r="O71" t="inlineStr"/>
       <c r="P71" t="n">
@@ -2779,7 +3445,15 @@
       <c r="J72" t="inlineStr"/>
       <c r="K72" t="inlineStr"/>
       <c r="L72" t="inlineStr"/>
-      <c r="M72" t="inlineStr"/>
+      <c r="M72" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q7 : RECHERCHE DES CAUSES
+Pour chaque écart relevé identifier faite une analyse des causes (en utilisant le diagramme 5M)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N72" t="inlineStr"/>
       <c r="O72" t="inlineStr"/>
       <c r="P72" t="n">
@@ -2811,7 +3485,17 @@
       <c r="J73" t="inlineStr"/>
       <c r="K73" t="inlineStr"/>
       <c r="L73" t="inlineStr"/>
-      <c r="M73" t="inlineStr"/>
+      <c r="M73" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q8 : SOLUTIONS
+Trouver 2 solutions pour chaque écart : 
+☞ Préciser à quelles causes elles correspondent
+☞ Décrire les solutions
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N73" t="inlineStr"/>
       <c r="O73" t="inlineStr"/>
       <c r="P73" t="n">
@@ -2843,7 +3527,17 @@
       <c r="J74" t="inlineStr"/>
       <c r="K74" t="inlineStr"/>
       <c r="L74" t="inlineStr"/>
-      <c r="M74" t="inlineStr"/>
+      <c r="M74" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q1 : ANALYSE DES RISQUES
+Quels sont les risques engendrés par cette situation
+Evaluer ces risques
+Identifier ceux qui sont critiques – et pourquoi (vous pouvez vous servir de la matrice de criticité des risques)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N74" t="inlineStr"/>
       <c r="O74" t="inlineStr"/>
       <c r="P74" t="n">
@@ -2875,7 +3569,17 @@
       <c r="J75" t="inlineStr"/>
       <c r="K75" t="inlineStr"/>
       <c r="L75" t="inlineStr"/>
-      <c r="M75" t="inlineStr"/>
+      <c r="M75" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q2 : DECLENCHEMENT DE L’AUDIT
+Qui mandate l’audit
+Qui va réaliser l’audit (vous pouvez choisir interne ou externe)
+Sur quels critères l’auditeur est choisi ?
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N75" t="inlineStr"/>
       <c r="O75" t="inlineStr"/>
       <c r="P75" t="n">
@@ -2907,7 +3611,17 @@
       <c r="J76" t="inlineStr"/>
       <c r="K76" t="inlineStr"/>
       <c r="L76" t="inlineStr"/>
-      <c r="M76" t="inlineStr"/>
+      <c r="M76" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q3 : PLANIFICATION DE L’AUDIT
+Quelles sont les étapes de l’audit
+Etablir le planning de l’audit (en tenant compte des dates prévues)
+Identifier les acteurs de l’audit et leurs responsabilités (utiliser la matrice RACI)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N76" t="inlineStr"/>
       <c r="O76" t="inlineStr"/>
       <c r="P76" t="n">
@@ -2939,7 +3653,15 @@
       <c r="J77" t="inlineStr"/>
       <c r="K77" t="inlineStr"/>
       <c r="L77" t="inlineStr"/>
-      <c r="M77" t="inlineStr"/>
+      <c r="M77" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q4 : ANALYSE DOCUMENTAIRE
+Quels sont les documents qui pourraient vous aider à préparer cet audit ? (Soyez précis, vous pouvez identifier des documents que DISTRELEC pourrait avoir)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N77" t="inlineStr"/>
       <c r="O77" t="inlineStr"/>
       <c r="P77" t="n">
@@ -2971,7 +3693,16 @@
       <c r="J78" t="inlineStr"/>
       <c r="K78" t="inlineStr"/>
       <c r="L78" t="inlineStr"/>
-      <c r="M78" t="inlineStr"/>
+      <c r="M78" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q5 : REALISATION DE L’AUDIT
+Identifier 3 personnes (fonctions) à auditer
+Elaborer le guide d’entretien pour l’un des audités (préciser lequel)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N78" t="inlineStr"/>
       <c r="O78" t="inlineStr"/>
       <c r="P78" t="n">
@@ -3003,7 +3734,18 @@
       <c r="J79" t="inlineStr"/>
       <c r="K79" t="inlineStr"/>
       <c r="L79" t="inlineStr"/>
-      <c r="M79" t="inlineStr"/>
+      <c r="M79" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q6 : CONCLUSIONS DE L’AUDIT
+Rédiger votre conclusion (à imaginer) présentant : 
+☞ 1 point fort
+☞ 2 points sensibles
+☞ 2 écarts
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N79" t="inlineStr"/>
       <c r="O79" t="inlineStr"/>
       <c r="P79" t="n">
@@ -3035,7 +3777,15 @@
       <c r="J80" t="inlineStr"/>
       <c r="K80" t="inlineStr"/>
       <c r="L80" t="inlineStr"/>
-      <c r="M80" t="inlineStr"/>
+      <c r="M80" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q7 : RECHERCHE DES CAUSES
+Pour chaque écart relevé identifier faite une analyse des causes (en utilisant le diagramme 5M)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N80" t="inlineStr"/>
       <c r="O80" t="inlineStr"/>
       <c r="P80" t="n">
@@ -3067,7 +3817,17 @@
       <c r="J81" t="inlineStr"/>
       <c r="K81" t="inlineStr"/>
       <c r="L81" t="inlineStr"/>
-      <c r="M81" t="inlineStr"/>
+      <c r="M81" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q8 : SOLUTIONS
+Trouver 2 solutions pour chaque écart : 
+☞ Préciser à quelles causes elles correspondent
+☞ Décrire les solutions
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N81" t="inlineStr"/>
       <c r="O81" t="inlineStr"/>
       <c r="P81" t="n">
@@ -3099,7 +3859,17 @@
       <c r="J82" t="inlineStr"/>
       <c r="K82" t="inlineStr"/>
       <c r="L82" t="inlineStr"/>
-      <c r="M82" t="inlineStr"/>
+      <c r="M82" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q1 : ANALYSE DES RISQUES
+Quels sont les risques engendrés par cette situation
+Evaluer ces risques
+Identifier ceux qui sont critiques – et pourquoi (vous pouvez vous servir de la matrice de criticité des risques)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N82" t="inlineStr"/>
       <c r="O82" t="inlineStr"/>
       <c r="P82" t="n">
@@ -3131,7 +3901,17 @@
       <c r="J83" t="inlineStr"/>
       <c r="K83" t="inlineStr"/>
       <c r="L83" t="inlineStr"/>
-      <c r="M83" t="inlineStr"/>
+      <c r="M83" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q2 : DECLENCHEMENT DE L’AUDIT
+Qui mandate l’audit
+Qui va réaliser l’audit (vous pouvez choisir interne ou externe)
+Sur quels critères l’auditeur est choisi ?
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N83" t="inlineStr"/>
       <c r="O83" t="inlineStr"/>
       <c r="P83" t="n">
@@ -3163,7 +3943,17 @@
       <c r="J84" t="inlineStr"/>
       <c r="K84" t="inlineStr"/>
       <c r="L84" t="inlineStr"/>
-      <c r="M84" t="inlineStr"/>
+      <c r="M84" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q3 : PLANIFICATION DE L’AUDIT
+Quelles sont les étapes de l’audit
+Etablir le planning de l’audit (en tenant compte des dates prévues)
+Identifier les acteurs de l’audit et leurs responsabilités (utiliser la matrice RACI)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N84" t="inlineStr"/>
       <c r="O84" t="inlineStr"/>
       <c r="P84" t="n">
@@ -3195,7 +3985,15 @@
       <c r="J85" t="inlineStr"/>
       <c r="K85" t="inlineStr"/>
       <c r="L85" t="inlineStr"/>
-      <c r="M85" t="inlineStr"/>
+      <c r="M85" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q4 : ANALYSE DOCUMENTAIRE
+Quels sont les documents qui pourraient vous aider à préparer cet audit ? (Soyez précis, vous pouvez identifier des documents que DISTRELEC pourrait avoir)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N85" t="inlineStr"/>
       <c r="O85" t="inlineStr"/>
       <c r="P85" t="n">
@@ -3227,7 +4025,16 @@
       <c r="J86" t="inlineStr"/>
       <c r="K86" t="inlineStr"/>
       <c r="L86" t="inlineStr"/>
-      <c r="M86" t="inlineStr"/>
+      <c r="M86" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q5 : REALISATION DE L’AUDIT
+Identifier 3 personnes (fonctions) à auditer
+Elaborer le guide d’entretien pour l’un des audités (préciser lequel)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N86" t="inlineStr"/>
       <c r="O86" t="inlineStr"/>
       <c r="P86" t="n">
@@ -3259,7 +4066,18 @@
       <c r="J87" t="inlineStr"/>
       <c r="K87" t="inlineStr"/>
       <c r="L87" t="inlineStr"/>
-      <c r="M87" t="inlineStr"/>
+      <c r="M87" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q6 : CONCLUSIONS DE L’AUDIT
+Rédiger votre conclusion (à imaginer) présentant : 
+☞ 1 point fort
+☞ 2 points sensibles
+☞ 2 écarts
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N87" t="inlineStr"/>
       <c r="O87" t="inlineStr"/>
       <c r="P87" t="n">
@@ -3291,7 +4109,15 @@
       <c r="J88" t="inlineStr"/>
       <c r="K88" t="inlineStr"/>
       <c r="L88" t="inlineStr"/>
-      <c r="M88" t="inlineStr"/>
+      <c r="M88" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q7 : RECHERCHE DES CAUSES
+Pour chaque écart relevé identifier faite une analyse des causes (en utilisant le diagramme 5M)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N88" t="inlineStr"/>
       <c r="O88" t="inlineStr"/>
       <c r="P88" t="n">
@@ -3323,7 +4149,17 @@
       <c r="J89" t="inlineStr"/>
       <c r="K89" t="inlineStr"/>
       <c r="L89" t="inlineStr"/>
-      <c r="M89" t="inlineStr"/>
+      <c r="M89" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q8 : SOLUTIONS
+Trouver 2 solutions pour chaque écart : 
+☞ Préciser à quelles causes elles correspondent
+☞ Décrire les solutions
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N89" t="inlineStr"/>
       <c r="O89" t="inlineStr"/>
       <c r="P89" t="n">
@@ -3355,7 +4191,17 @@
       <c r="J90" t="inlineStr"/>
       <c r="K90" t="inlineStr"/>
       <c r="L90" t="inlineStr"/>
-      <c r="M90" t="inlineStr"/>
+      <c r="M90" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q1 : ANALYSE DES RISQUES
+Quels sont les risques engendrés par cette situation
+Evaluer ces risques
+Identifier ceux qui sont critiques – et pourquoi (vous pouvez vous servir de la matrice de criticité des risques)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N90" t="inlineStr"/>
       <c r="O90" t="inlineStr"/>
       <c r="P90" t="n">
@@ -3387,7 +4233,17 @@
       <c r="J91" t="inlineStr"/>
       <c r="K91" t="inlineStr"/>
       <c r="L91" t="inlineStr"/>
-      <c r="M91" t="inlineStr"/>
+      <c r="M91" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q2 : DECLENCHEMENT DE L’AUDIT
+Qui mandate l’audit
+Qui va réaliser l’audit (vous pouvez choisir interne ou externe)
+Sur quels critères l’auditeur est choisi ?
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N91" t="inlineStr"/>
       <c r="O91" t="inlineStr"/>
       <c r="P91" t="n">
@@ -3419,7 +4275,17 @@
       <c r="J92" t="inlineStr"/>
       <c r="K92" t="inlineStr"/>
       <c r="L92" t="inlineStr"/>
-      <c r="M92" t="inlineStr"/>
+      <c r="M92" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q3 : PLANIFICATION DE L’AUDIT
+Quelles sont les étapes de l’audit
+Etablir le planning de l’audit (en tenant compte des dates prévues)
+Identifier les acteurs de l’audit et leurs responsabilités (utiliser la matrice RACI)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N92" t="inlineStr"/>
       <c r="O92" t="inlineStr"/>
       <c r="P92" t="n">
@@ -3451,7 +4317,15 @@
       <c r="J93" t="inlineStr"/>
       <c r="K93" t="inlineStr"/>
       <c r="L93" t="inlineStr"/>
-      <c r="M93" t="inlineStr"/>
+      <c r="M93" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q4 : ANALYSE DOCUMENTAIRE
+Quels sont les documents qui pourraient vous aider à préparer cet audit ? (Soyez précis, vous pouvez identifier des documents que DISTRELEC pourrait avoir)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N93" t="inlineStr"/>
       <c r="O93" t="inlineStr"/>
       <c r="P93" t="n">
@@ -3483,7 +4357,16 @@
       <c r="J94" t="inlineStr"/>
       <c r="K94" t="inlineStr"/>
       <c r="L94" t="inlineStr"/>
-      <c r="M94" t="inlineStr"/>
+      <c r="M94" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q5 : REALISATION DE L’AUDIT
+Identifier 3 personnes (fonctions) à auditer
+Elaborer le guide d’entretien pour l’un des audités (préciser lequel)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N94" t="inlineStr"/>
       <c r="O94" t="inlineStr"/>
       <c r="P94" t="n">
@@ -3515,7 +4398,18 @@
       <c r="J95" t="inlineStr"/>
       <c r="K95" t="inlineStr"/>
       <c r="L95" t="inlineStr"/>
-      <c r="M95" t="inlineStr"/>
+      <c r="M95" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q6 : CONCLUSIONS DE L’AUDIT
+Rédiger votre conclusion (à imaginer) présentant : 
+☞ 1 point fort
+☞ 2 points sensibles
+☞ 2 écarts
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N95" t="inlineStr"/>
       <c r="O95" t="inlineStr"/>
       <c r="P95" t="n">
@@ -3547,7 +4441,15 @@
       <c r="J96" t="inlineStr"/>
       <c r="K96" t="inlineStr"/>
       <c r="L96" t="inlineStr"/>
-      <c r="M96" t="inlineStr"/>
+      <c r="M96" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q7 : RECHERCHE DES CAUSES
+Pour chaque écart relevé identifier faite une analyse des causes (en utilisant le diagramme 5M)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N96" t="inlineStr"/>
       <c r="O96" t="inlineStr"/>
       <c r="P96" t="n">
@@ -3579,7 +4481,17 @@
       <c r="J97" t="inlineStr"/>
       <c r="K97" t="inlineStr"/>
       <c r="L97" t="inlineStr"/>
-      <c r="M97" t="inlineStr"/>
+      <c r="M97" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q8 : SOLUTIONS
+Trouver 2 solutions pour chaque écart : 
+☞ Préciser à quelles causes elles correspondent
+☞ Décrire les solutions
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N97" t="inlineStr"/>
       <c r="O97" t="inlineStr"/>
       <c r="P97" t="n">
@@ -3611,7 +4523,17 @@
       <c r="J98" t="inlineStr"/>
       <c r="K98" t="inlineStr"/>
       <c r="L98" t="inlineStr"/>
-      <c r="M98" t="inlineStr"/>
+      <c r="M98" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q1 : ANALYSE DES RISQUES
+Quels sont les risques engendrés par cette situation
+Evaluer ces risques
+Identifier ceux qui sont critiques – et pourquoi (vous pouvez vous servir de la matrice de criticité des risques)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N98" t="inlineStr"/>
       <c r="O98" t="inlineStr"/>
       <c r="P98" t="n">
@@ -3643,7 +4565,17 @@
       <c r="J99" t="inlineStr"/>
       <c r="K99" t="inlineStr"/>
       <c r="L99" t="inlineStr"/>
-      <c r="M99" t="inlineStr"/>
+      <c r="M99" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q2 : DECLENCHEMENT DE L’AUDIT
+Qui mandate l’audit
+Qui va réaliser l’audit (vous pouvez choisir interne ou externe)
+Sur quels critères l’auditeur est choisi ?
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N99" t="inlineStr"/>
       <c r="O99" t="inlineStr"/>
       <c r="P99" t="n">
@@ -3675,7 +4607,17 @@
       <c r="J100" t="inlineStr"/>
       <c r="K100" t="inlineStr"/>
       <c r="L100" t="inlineStr"/>
-      <c r="M100" t="inlineStr"/>
+      <c r="M100" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q3 : PLANIFICATION DE L’AUDIT
+Quelles sont les étapes de l’audit
+Etablir le planning de l’audit (en tenant compte des dates prévues)
+Identifier les acteurs de l’audit et leurs responsabilités (utiliser la matrice RACI)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N100" t="inlineStr"/>
       <c r="O100" t="inlineStr"/>
       <c r="P100" t="n">
@@ -3707,7 +4649,15 @@
       <c r="J101" t="inlineStr"/>
       <c r="K101" t="inlineStr"/>
       <c r="L101" t="inlineStr"/>
-      <c r="M101" t="inlineStr"/>
+      <c r="M101" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q4 : ANALYSE DOCUMENTAIRE
+Quels sont les documents qui pourraient vous aider à préparer cet audit ? (Soyez précis, vous pouvez identifier des documents que DISTRELEC pourrait avoir)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N101" t="inlineStr"/>
       <c r="O101" t="inlineStr"/>
       <c r="P101" t="n">
@@ -3739,7 +4689,16 @@
       <c r="J102" t="inlineStr"/>
       <c r="K102" t="inlineStr"/>
       <c r="L102" t="inlineStr"/>
-      <c r="M102" t="inlineStr"/>
+      <c r="M102" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q5 : REALISATION DE L’AUDIT
+Identifier 3 personnes (fonctions) à auditer
+Elaborer le guide d’entretien pour l’un des audités (préciser lequel)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N102" t="inlineStr"/>
       <c r="O102" t="inlineStr"/>
       <c r="P102" t="n">
@@ -3771,7 +4730,18 @@
       <c r="J103" t="inlineStr"/>
       <c r="K103" t="inlineStr"/>
       <c r="L103" t="inlineStr"/>
-      <c r="M103" t="inlineStr"/>
+      <c r="M103" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q6 : CONCLUSIONS DE L’AUDIT
+Rédiger votre conclusion (à imaginer) présentant : 
+☞ 1 point fort
+☞ 2 points sensibles
+☞ 2 écarts
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N103" t="inlineStr"/>
       <c r="O103" t="inlineStr"/>
       <c r="P103" t="n">
@@ -3803,7 +4773,15 @@
       <c r="J104" t="inlineStr"/>
       <c r="K104" t="inlineStr"/>
       <c r="L104" t="inlineStr"/>
-      <c r="M104" t="inlineStr"/>
+      <c r="M104" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q7 : RECHERCHE DES CAUSES
+Pour chaque écart relevé identifier faite une analyse des causes (en utilisant le diagramme 5M)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N104" t="inlineStr"/>
       <c r="O104" t="inlineStr"/>
       <c r="P104" t="n">
@@ -3835,7 +4813,17 @@
       <c r="J105" t="inlineStr"/>
       <c r="K105" t="inlineStr"/>
       <c r="L105" t="inlineStr"/>
-      <c r="M105" t="inlineStr"/>
+      <c r="M105" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q8 : SOLUTIONS
+Trouver 2 solutions pour chaque écart : 
+☞ Préciser à quelles causes elles correspondent
+☞ Décrire les solutions
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N105" t="inlineStr"/>
       <c r="O105" t="inlineStr"/>
       <c r="P105" t="n">
@@ -3867,7 +4855,17 @@
       <c r="J106" t="inlineStr"/>
       <c r="K106" t="inlineStr"/>
       <c r="L106" t="inlineStr"/>
-      <c r="M106" t="inlineStr"/>
+      <c r="M106" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q1 : ANALYSE DES RISQUES
+Quels sont les risques engendrés par cette situation
+Evaluer ces risques
+Identifier ceux qui sont critiques – et pourquoi (vous pouvez vous servir de la matrice de criticité des risques)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N106" t="inlineStr"/>
       <c r="O106" t="inlineStr"/>
       <c r="P106" t="n">
@@ -3899,7 +4897,17 @@
       <c r="J107" t="inlineStr"/>
       <c r="K107" t="inlineStr"/>
       <c r="L107" t="inlineStr"/>
-      <c r="M107" t="inlineStr"/>
+      <c r="M107" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q2 : DECLENCHEMENT DE L’AUDIT
+Qui mandate l’audit
+Qui va réaliser l’audit (vous pouvez choisir interne ou externe)
+Sur quels critères l’auditeur est choisi ?
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N107" t="inlineStr"/>
       <c r="O107" t="inlineStr"/>
       <c r="P107" t="n">
@@ -3931,7 +4939,17 @@
       <c r="J108" t="inlineStr"/>
       <c r="K108" t="inlineStr"/>
       <c r="L108" t="inlineStr"/>
-      <c r="M108" t="inlineStr"/>
+      <c r="M108" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q3 : PLANIFICATION DE L’AUDIT
+Quelles sont les étapes de l’audit
+Etablir le planning de l’audit (en tenant compte des dates prévues)
+Identifier les acteurs de l’audit et leurs responsabilités (utiliser la matrice RACI)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N108" t="inlineStr"/>
       <c r="O108" t="inlineStr"/>
       <c r="P108" t="n">
@@ -3963,7 +4981,15 @@
       <c r="J109" t="inlineStr"/>
       <c r="K109" t="inlineStr"/>
       <c r="L109" t="inlineStr"/>
-      <c r="M109" t="inlineStr"/>
+      <c r="M109" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q4 : ANALYSE DOCUMENTAIRE
+Quels sont les documents qui pourraient vous aider à préparer cet audit ? (Soyez précis, vous pouvez identifier des documents que DISTRELEC pourrait avoir)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N109" t="inlineStr"/>
       <c r="O109" t="inlineStr"/>
       <c r="P109" t="n">
@@ -3995,7 +5021,16 @@
       <c r="J110" t="inlineStr"/>
       <c r="K110" t="inlineStr"/>
       <c r="L110" t="inlineStr"/>
-      <c r="M110" t="inlineStr"/>
+      <c r="M110" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q5 : REALISATION DE L’AUDIT
+Identifier 3 personnes (fonctions) à auditer
+Elaborer le guide d’entretien pour l’un des audités (préciser lequel)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N110" t="inlineStr"/>
       <c r="O110" t="inlineStr"/>
       <c r="P110" t="n">
@@ -4027,7 +5062,18 @@
       <c r="J111" t="inlineStr"/>
       <c r="K111" t="inlineStr"/>
       <c r="L111" t="inlineStr"/>
-      <c r="M111" t="inlineStr"/>
+      <c r="M111" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q6 : CONCLUSIONS DE L’AUDIT
+Rédiger votre conclusion (à imaginer) présentant : 
+☞ 1 point fort
+☞ 2 points sensibles
+☞ 2 écarts
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N111" t="inlineStr"/>
       <c r="O111" t="inlineStr"/>
       <c r="P111" t="n">
@@ -4059,7 +5105,15 @@
       <c r="J112" t="inlineStr"/>
       <c r="K112" t="inlineStr"/>
       <c r="L112" t="inlineStr"/>
-      <c r="M112" t="inlineStr"/>
+      <c r="M112" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q7 : RECHERCHE DES CAUSES
+Pour chaque écart relevé identifier faite une analyse des causes (en utilisant le diagramme 5M)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N112" t="inlineStr"/>
       <c r="O112" t="inlineStr"/>
       <c r="P112" t="n">
@@ -4091,7 +5145,17 @@
       <c r="J113" t="inlineStr"/>
       <c r="K113" t="inlineStr"/>
       <c r="L113" t="inlineStr"/>
-      <c r="M113" t="inlineStr"/>
+      <c r="M113" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q8 : SOLUTIONS
+Trouver 2 solutions pour chaque écart : 
+☞ Préciser à quelles causes elles correspondent
+☞ Décrire les solutions
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N113" t="inlineStr"/>
       <c r="O113" t="inlineStr"/>
       <c r="P113" t="n">
@@ -4123,7 +5187,17 @@
       <c r="J114" t="inlineStr"/>
       <c r="K114" t="inlineStr"/>
       <c r="L114" t="inlineStr"/>
-      <c r="M114" t="inlineStr"/>
+      <c r="M114" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q1 : ANALYSE DES RISQUES
+Quels sont les risques engendrés par cette situation
+Evaluer ces risques
+Identifier ceux qui sont critiques – et pourquoi (vous pouvez vous servir de la matrice de criticité des risques)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N114" t="inlineStr"/>
       <c r="O114" t="inlineStr"/>
       <c r="P114" t="n">
@@ -4155,7 +5229,17 @@
       <c r="J115" t="inlineStr"/>
       <c r="K115" t="inlineStr"/>
       <c r="L115" t="inlineStr"/>
-      <c r="M115" t="inlineStr"/>
+      <c r="M115" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q2 : DECLENCHEMENT DE L’AUDIT
+Qui mandate l’audit
+Qui va réaliser l’audit (vous pouvez choisir interne ou externe)
+Sur quels critères l’auditeur est choisi ?
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N115" t="inlineStr"/>
       <c r="O115" t="inlineStr"/>
       <c r="P115" t="n">
@@ -4187,7 +5271,17 @@
       <c r="J116" t="inlineStr"/>
       <c r="K116" t="inlineStr"/>
       <c r="L116" t="inlineStr"/>
-      <c r="M116" t="inlineStr"/>
+      <c r="M116" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q3 : PLANIFICATION DE L’AUDIT
+Quelles sont les étapes de l’audit
+Etablir le planning de l’audit (en tenant compte des dates prévues)
+Identifier les acteurs de l’audit et leurs responsabilités (utiliser la matrice RACI)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N116" t="inlineStr"/>
       <c r="O116" t="inlineStr"/>
       <c r="P116" t="n">
@@ -4219,7 +5313,15 @@
       <c r="J117" t="inlineStr"/>
       <c r="K117" t="inlineStr"/>
       <c r="L117" t="inlineStr"/>
-      <c r="M117" t="inlineStr"/>
+      <c r="M117" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q4 : ANALYSE DOCUMENTAIRE
+Quels sont les documents qui pourraient vous aider à préparer cet audit ? (Soyez précis, vous pouvez identifier des documents que DISTRELEC pourrait avoir)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N117" t="inlineStr"/>
       <c r="O117" t="inlineStr"/>
       <c r="P117" t="n">
@@ -4251,7 +5353,16 @@
       <c r="J118" t="inlineStr"/>
       <c r="K118" t="inlineStr"/>
       <c r="L118" t="inlineStr"/>
-      <c r="M118" t="inlineStr"/>
+      <c r="M118" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q5 : REALISATION DE L’AUDIT
+Identifier 3 personnes (fonctions) à auditer
+Elaborer le guide d’entretien pour l’un des audités (préciser lequel)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N118" t="inlineStr"/>
       <c r="O118" t="inlineStr"/>
       <c r="P118" t="n">
@@ -4283,7 +5394,18 @@
       <c r="J119" t="inlineStr"/>
       <c r="K119" t="inlineStr"/>
       <c r="L119" t="inlineStr"/>
-      <c r="M119" t="inlineStr"/>
+      <c r="M119" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q6 : CONCLUSIONS DE L’AUDIT
+Rédiger votre conclusion (à imaginer) présentant : 
+☞ 1 point fort
+☞ 2 points sensibles
+☞ 2 écarts
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N119" t="inlineStr"/>
       <c r="O119" t="inlineStr"/>
       <c r="P119" t="n">
@@ -4315,7 +5437,15 @@
       <c r="J120" t="inlineStr"/>
       <c r="K120" t="inlineStr"/>
       <c r="L120" t="inlineStr"/>
-      <c r="M120" t="inlineStr"/>
+      <c r="M120" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q7 : RECHERCHE DES CAUSES
+Pour chaque écart relevé identifier faite une analyse des causes (en utilisant le diagramme 5M)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N120" t="inlineStr"/>
       <c r="O120" t="inlineStr"/>
       <c r="P120" t="n">
@@ -4347,7 +5477,17 @@
       <c r="J121" t="inlineStr"/>
       <c r="K121" t="inlineStr"/>
       <c r="L121" t="inlineStr"/>
-      <c r="M121" t="inlineStr"/>
+      <c r="M121" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q8 : SOLUTIONS
+Trouver 2 solutions pour chaque écart : 
+☞ Préciser à quelles causes elles correspondent
+☞ Décrire les solutions
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N121" t="inlineStr"/>
       <c r="O121" t="inlineStr"/>
       <c r="P121" t="n">
@@ -4379,7 +5519,17 @@
       <c r="J122" t="inlineStr"/>
       <c r="K122" t="inlineStr"/>
       <c r="L122" t="inlineStr"/>
-      <c r="M122" t="inlineStr"/>
+      <c r="M122" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q1 : ANALYSE DES RISQUES
+Quels sont les risques engendrés par cette situation
+Evaluer ces risques
+Identifier ceux qui sont critiques – et pourquoi (vous pouvez vous servir de la matrice de criticité des risques)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N122" t="inlineStr"/>
       <c r="O122" t="inlineStr"/>
       <c r="P122" t="n">
@@ -4411,7 +5561,17 @@
       <c r="J123" t="inlineStr"/>
       <c r="K123" t="inlineStr"/>
       <c r="L123" t="inlineStr"/>
-      <c r="M123" t="inlineStr"/>
+      <c r="M123" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q2 : DECLENCHEMENT DE L’AUDIT
+Qui mandate l’audit
+Qui va réaliser l’audit (vous pouvez choisir interne ou externe)
+Sur quels critères l’auditeur est choisi ?
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N123" t="inlineStr"/>
       <c r="O123" t="inlineStr"/>
       <c r="P123" t="n">
@@ -4443,7 +5603,17 @@
       <c r="J124" t="inlineStr"/>
       <c r="K124" t="inlineStr"/>
       <c r="L124" t="inlineStr"/>
-      <c r="M124" t="inlineStr"/>
+      <c r="M124" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q3 : PLANIFICATION DE L’AUDIT
+Quelles sont les étapes de l’audit
+Etablir le planning de l’audit (en tenant compte des dates prévues)
+Identifier les acteurs de l’audit et leurs responsabilités (utiliser la matrice RACI)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N124" t="inlineStr"/>
       <c r="O124" t="inlineStr"/>
       <c r="P124" t="n">
@@ -4475,7 +5645,15 @@
       <c r="J125" t="inlineStr"/>
       <c r="K125" t="inlineStr"/>
       <c r="L125" t="inlineStr"/>
-      <c r="M125" t="inlineStr"/>
+      <c r="M125" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q4 : ANALYSE DOCUMENTAIRE
+Quels sont les documents qui pourraient vous aider à préparer cet audit ? (Soyez précis, vous pouvez identifier des documents que DISTRELEC pourrait avoir)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N125" t="inlineStr"/>
       <c r="O125" t="inlineStr"/>
       <c r="P125" t="n">
@@ -4507,7 +5685,16 @@
       <c r="J126" t="inlineStr"/>
       <c r="K126" t="inlineStr"/>
       <c r="L126" t="inlineStr"/>
-      <c r="M126" t="inlineStr"/>
+      <c r="M126" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q5 : REALISATION DE L’AUDIT
+Identifier 3 personnes (fonctions) à auditer
+Elaborer le guide d’entretien pour l’un des audités (préciser lequel)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N126" t="inlineStr"/>
       <c r="O126" t="inlineStr"/>
       <c r="P126" t="n">
@@ -4539,7 +5726,18 @@
       <c r="J127" t="inlineStr"/>
       <c r="K127" t="inlineStr"/>
       <c r="L127" t="inlineStr"/>
-      <c r="M127" t="inlineStr"/>
+      <c r="M127" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q6 : CONCLUSIONS DE L’AUDIT
+Rédiger votre conclusion (à imaginer) présentant : 
+☞ 1 point fort
+☞ 2 points sensibles
+☞ 2 écarts
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N127" t="inlineStr"/>
       <c r="O127" t="inlineStr"/>
       <c r="P127" t="n">
@@ -4571,7 +5769,15 @@
       <c r="J128" t="inlineStr"/>
       <c r="K128" t="inlineStr"/>
       <c r="L128" t="inlineStr"/>
-      <c r="M128" t="inlineStr"/>
+      <c r="M128" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q7 : RECHERCHE DES CAUSES
+Pour chaque écart relevé identifier faite une analyse des causes (en utilisant le diagramme 5M)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N128" t="inlineStr"/>
       <c r="O128" t="inlineStr"/>
       <c r="P128" t="n">
@@ -4603,7 +5809,17 @@
       <c r="J129" t="inlineStr"/>
       <c r="K129" t="inlineStr"/>
       <c r="L129" t="inlineStr"/>
-      <c r="M129" t="inlineStr"/>
+      <c r="M129" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q8 : SOLUTIONS
+Trouver 2 solutions pour chaque écart : 
+☞ Préciser à quelles causes elles correspondent
+☞ Décrire les solutions
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N129" t="inlineStr"/>
       <c r="O129" t="inlineStr"/>
       <c r="P129" t="n">
@@ -4635,7 +5851,17 @@
       <c r="J130" t="inlineStr"/>
       <c r="K130" t="inlineStr"/>
       <c r="L130" t="inlineStr"/>
-      <c r="M130" t="inlineStr"/>
+      <c r="M130" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q1 : ANALYSE DES RISQUES
+Quels sont les risques engendrés par cette situation
+Evaluer ces risques
+Identifier ceux qui sont critiques – et pourquoi (vous pouvez vous servir de la matrice de criticité des risques)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N130" t="inlineStr"/>
       <c r="O130" t="inlineStr"/>
       <c r="P130" t="n">
@@ -4667,7 +5893,17 @@
       <c r="J131" t="inlineStr"/>
       <c r="K131" t="inlineStr"/>
       <c r="L131" t="inlineStr"/>
-      <c r="M131" t="inlineStr"/>
+      <c r="M131" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q2 : DECLENCHEMENT DE L’AUDIT
+Qui mandate l’audit
+Qui va réaliser l’audit (vous pouvez choisir interne ou externe)
+Sur quels critères l’auditeur est choisi ?
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N131" t="inlineStr"/>
       <c r="O131" t="inlineStr"/>
       <c r="P131" t="n">
@@ -4699,7 +5935,17 @@
       <c r="J132" t="inlineStr"/>
       <c r="K132" t="inlineStr"/>
       <c r="L132" t="inlineStr"/>
-      <c r="M132" t="inlineStr"/>
+      <c r="M132" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q3 : PLANIFICATION DE L’AUDIT
+Quelles sont les étapes de l’audit
+Etablir le planning de l’audit (en tenant compte des dates prévues)
+Identifier les acteurs de l’audit et leurs responsabilités (utiliser la matrice RACI)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N132" t="inlineStr"/>
       <c r="O132" t="inlineStr"/>
       <c r="P132" t="n">
@@ -4731,7 +5977,15 @@
       <c r="J133" t="inlineStr"/>
       <c r="K133" t="inlineStr"/>
       <c r="L133" t="inlineStr"/>
-      <c r="M133" t="inlineStr"/>
+      <c r="M133" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q4 : ANALYSE DOCUMENTAIRE
+Quels sont les documents qui pourraient vous aider à préparer cet audit ? (Soyez précis, vous pouvez identifier des documents que DISTRELEC pourrait avoir)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N133" t="inlineStr"/>
       <c r="O133" t="inlineStr"/>
       <c r="P133" t="n">
@@ -4763,7 +6017,16 @@
       <c r="J134" t="inlineStr"/>
       <c r="K134" t="inlineStr"/>
       <c r="L134" t="inlineStr"/>
-      <c r="M134" t="inlineStr"/>
+      <c r="M134" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q5 : REALISATION DE L’AUDIT
+Identifier 3 personnes (fonctions) à auditer
+Elaborer le guide d’entretien pour l’un des audités (préciser lequel)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N134" t="inlineStr"/>
       <c r="O134" t="inlineStr"/>
       <c r="P134" t="n">
@@ -4795,7 +6058,18 @@
       <c r="J135" t="inlineStr"/>
       <c r="K135" t="inlineStr"/>
       <c r="L135" t="inlineStr"/>
-      <c r="M135" t="inlineStr"/>
+      <c r="M135" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q6 : CONCLUSIONS DE L’AUDIT
+Rédiger votre conclusion (à imaginer) présentant : 
+☞ 1 point fort
+☞ 2 points sensibles
+☞ 2 écarts
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N135" t="inlineStr"/>
       <c r="O135" t="inlineStr"/>
       <c r="P135" t="n">
@@ -4827,7 +6101,15 @@
       <c r="J136" t="inlineStr"/>
       <c r="K136" t="inlineStr"/>
       <c r="L136" t="inlineStr"/>
-      <c r="M136" t="inlineStr"/>
+      <c r="M136" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q7 : RECHERCHE DES CAUSES
+Pour chaque écart relevé identifier faite une analyse des causes (en utilisant le diagramme 5M)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N136" t="inlineStr"/>
       <c r="O136" t="inlineStr"/>
       <c r="P136" t="n">
@@ -4859,7 +6141,17 @@
       <c r="J137" t="inlineStr"/>
       <c r="K137" t="inlineStr"/>
       <c r="L137" t="inlineStr"/>
-      <c r="M137" t="inlineStr"/>
+      <c r="M137" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q8 : SOLUTIONS
+Trouver 2 solutions pour chaque écart : 
+☞ Préciser à quelles causes elles correspondent
+☞ Décrire les solutions
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N137" t="inlineStr"/>
       <c r="O137" t="inlineStr"/>
       <c r="P137" t="n">
@@ -4891,7 +6183,17 @@
       <c r="J138" t="inlineStr"/>
       <c r="K138" t="inlineStr"/>
       <c r="L138" t="inlineStr"/>
-      <c r="M138" t="inlineStr"/>
+      <c r="M138" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q1 : ANALYSE DES RISQUES
+Quels sont les risques engendrés par cette situation
+Evaluer ces risques
+Identifier ceux qui sont critiques – et pourquoi (vous pouvez vous servir de la matrice de criticité des risques)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N138" t="inlineStr"/>
       <c r="O138" t="inlineStr"/>
       <c r="P138" t="n">
@@ -4923,7 +6225,17 @@
       <c r="J139" t="inlineStr"/>
       <c r="K139" t="inlineStr"/>
       <c r="L139" t="inlineStr"/>
-      <c r="M139" t="inlineStr"/>
+      <c r="M139" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q2 : DECLENCHEMENT DE L’AUDIT
+Qui mandate l’audit
+Qui va réaliser l’audit (vous pouvez choisir interne ou externe)
+Sur quels critères l’auditeur est choisi ?
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N139" t="inlineStr"/>
       <c r="O139" t="inlineStr"/>
       <c r="P139" t="n">
@@ -4955,7 +6267,17 @@
       <c r="J140" t="inlineStr"/>
       <c r="K140" t="inlineStr"/>
       <c r="L140" t="inlineStr"/>
-      <c r="M140" t="inlineStr"/>
+      <c r="M140" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q3 : PLANIFICATION DE L’AUDIT
+Quelles sont les étapes de l’audit
+Etablir le planning de l’audit (en tenant compte des dates prévues)
+Identifier les acteurs de l’audit et leurs responsabilités (utiliser la matrice RACI)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N140" t="inlineStr"/>
       <c r="O140" t="inlineStr"/>
       <c r="P140" t="n">
@@ -4987,7 +6309,15 @@
       <c r="J141" t="inlineStr"/>
       <c r="K141" t="inlineStr"/>
       <c r="L141" t="inlineStr"/>
-      <c r="M141" t="inlineStr"/>
+      <c r="M141" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q4 : ANALYSE DOCUMENTAIRE
+Quels sont les documents qui pourraient vous aider à préparer cet audit ? (Soyez précis, vous pouvez identifier des documents que DISTRELEC pourrait avoir)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N141" t="inlineStr"/>
       <c r="O141" t="inlineStr"/>
       <c r="P141" t="n">
@@ -5019,7 +6349,16 @@
       <c r="J142" t="inlineStr"/>
       <c r="K142" t="inlineStr"/>
       <c r="L142" t="inlineStr"/>
-      <c r="M142" t="inlineStr"/>
+      <c r="M142" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q5 : REALISATION DE L’AUDIT
+Identifier 3 personnes (fonctions) à auditer
+Elaborer le guide d’entretien pour l’un des audités (préciser lequel)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N142" t="inlineStr"/>
       <c r="O142" t="inlineStr"/>
       <c r="P142" t="n">
@@ -5051,7 +6390,18 @@
       <c r="J143" t="inlineStr"/>
       <c r="K143" t="inlineStr"/>
       <c r="L143" t="inlineStr"/>
-      <c r="M143" t="inlineStr"/>
+      <c r="M143" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q6 : CONCLUSIONS DE L’AUDIT
+Rédiger votre conclusion (à imaginer) présentant : 
+☞ 1 point fort
+☞ 2 points sensibles
+☞ 2 écarts
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N143" t="inlineStr"/>
       <c r="O143" t="inlineStr"/>
       <c r="P143" t="n">
@@ -5083,7 +6433,15 @@
       <c r="J144" t="inlineStr"/>
       <c r="K144" t="inlineStr"/>
       <c r="L144" t="inlineStr"/>
-      <c r="M144" t="inlineStr"/>
+      <c r="M144" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q7 : RECHERCHE DES CAUSES
+Pour chaque écart relevé identifier faite une analyse des causes (en utilisant le diagramme 5M)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N144" t="inlineStr"/>
       <c r="O144" t="inlineStr"/>
       <c r="P144" t="n">
@@ -5115,7 +6473,17 @@
       <c r="J145" t="inlineStr"/>
       <c r="K145" t="inlineStr"/>
       <c r="L145" t="inlineStr"/>
-      <c r="M145" t="inlineStr"/>
+      <c r="M145" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q8 : SOLUTIONS
+Trouver 2 solutions pour chaque écart : 
+☞ Préciser à quelles causes elles correspondent
+☞ Décrire les solutions
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N145" t="inlineStr"/>
       <c r="O145" t="inlineStr"/>
       <c r="P145" t="n">
@@ -5147,7 +6515,17 @@
       <c r="J146" t="inlineStr"/>
       <c r="K146" t="inlineStr"/>
       <c r="L146" t="inlineStr"/>
-      <c r="M146" t="inlineStr"/>
+      <c r="M146" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q1 : ANALYSE DES RISQUES
+Quels sont les risques engendrés par cette situation
+Evaluer ces risques
+Identifier ceux qui sont critiques – et pourquoi (vous pouvez vous servir de la matrice de criticité des risques)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N146" t="inlineStr"/>
       <c r="O146" t="inlineStr"/>
       <c r="P146" t="n">
@@ -5179,7 +6557,17 @@
       <c r="J147" t="inlineStr"/>
       <c r="K147" t="inlineStr"/>
       <c r="L147" t="inlineStr"/>
-      <c r="M147" t="inlineStr"/>
+      <c r="M147" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q2 : DECLENCHEMENT DE L’AUDIT
+Qui mandate l’audit
+Qui va réaliser l’audit (vous pouvez choisir interne ou externe)
+Sur quels critères l’auditeur est choisi ?
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N147" t="inlineStr"/>
       <c r="O147" t="inlineStr"/>
       <c r="P147" t="n">
@@ -5211,7 +6599,17 @@
       <c r="J148" t="inlineStr"/>
       <c r="K148" t="inlineStr"/>
       <c r="L148" t="inlineStr"/>
-      <c r="M148" t="inlineStr"/>
+      <c r="M148" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q3 : PLANIFICATION DE L’AUDIT
+Quelles sont les étapes de l’audit
+Etablir le planning de l’audit (en tenant compte des dates prévues)
+Identifier les acteurs de l’audit et leurs responsabilités (utiliser la matrice RACI)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N148" t="inlineStr"/>
       <c r="O148" t="inlineStr"/>
       <c r="P148" t="n">
@@ -5243,7 +6641,15 @@
       <c r="J149" t="inlineStr"/>
       <c r="K149" t="inlineStr"/>
       <c r="L149" t="inlineStr"/>
-      <c r="M149" t="inlineStr"/>
+      <c r="M149" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q4 : ANALYSE DOCUMENTAIRE
+Quels sont les documents qui pourraient vous aider à préparer cet audit ? (Soyez précis, vous pouvez identifier des documents que DISTRELEC pourrait avoir)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N149" t="inlineStr"/>
       <c r="O149" t="inlineStr"/>
       <c r="P149" t="n">
@@ -5275,7 +6681,16 @@
       <c r="J150" t="inlineStr"/>
       <c r="K150" t="inlineStr"/>
       <c r="L150" t="inlineStr"/>
-      <c r="M150" t="inlineStr"/>
+      <c r="M150" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q5 : REALISATION DE L’AUDIT
+Identifier 3 personnes (fonctions) à auditer
+Elaborer le guide d’entretien pour l’un des audités (préciser lequel)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N150" t="inlineStr"/>
       <c r="O150" t="inlineStr"/>
       <c r="P150" t="n">
@@ -5307,7 +6722,18 @@
       <c r="J151" t="inlineStr"/>
       <c r="K151" t="inlineStr"/>
       <c r="L151" t="inlineStr"/>
-      <c r="M151" t="inlineStr"/>
+      <c r="M151" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q6 : CONCLUSIONS DE L’AUDIT
+Rédiger votre conclusion (à imaginer) présentant : 
+☞ 1 point fort
+☞ 2 points sensibles
+☞ 2 écarts
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N151" t="inlineStr"/>
       <c r="O151" t="inlineStr"/>
       <c r="P151" t="n">
@@ -5339,7 +6765,15 @@
       <c r="J152" t="inlineStr"/>
       <c r="K152" t="inlineStr"/>
       <c r="L152" t="inlineStr"/>
-      <c r="M152" t="inlineStr"/>
+      <c r="M152" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q7 : RECHERCHE DES CAUSES
+Pour chaque écart relevé identifier faite une analyse des causes (en utilisant le diagramme 5M)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N152" t="inlineStr"/>
       <c r="O152" t="inlineStr"/>
       <c r="P152" t="n">
@@ -5371,7 +6805,17 @@
       <c r="J153" t="inlineStr"/>
       <c r="K153" t="inlineStr"/>
       <c r="L153" t="inlineStr"/>
-      <c r="M153" t="inlineStr"/>
+      <c r="M153" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q8 : SOLUTIONS
+Trouver 2 solutions pour chaque écart : 
+☞ Préciser à quelles causes elles correspondent
+☞ Décrire les solutions
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N153" t="inlineStr"/>
       <c r="O153" t="inlineStr"/>
       <c r="P153" t="n">
@@ -5403,7 +6847,17 @@
       <c r="J154" t="inlineStr"/>
       <c r="K154" t="inlineStr"/>
       <c r="L154" t="inlineStr"/>
-      <c r="M154" t="inlineStr"/>
+      <c r="M154" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q1 : ANALYSE DES RISQUES
+Quels sont les risques engendrés par cette situation
+Evaluer ces risques
+Identifier ceux qui sont critiques – et pourquoi (vous pouvez vous servir de la matrice de criticité des risques)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N154" t="inlineStr"/>
       <c r="O154" t="inlineStr"/>
       <c r="P154" t="n">
@@ -5435,7 +6889,17 @@
       <c r="J155" t="inlineStr"/>
       <c r="K155" t="inlineStr"/>
       <c r="L155" t="inlineStr"/>
-      <c r="M155" t="inlineStr"/>
+      <c r="M155" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q2 : DECLENCHEMENT DE L’AUDIT
+Qui mandate l’audit
+Qui va réaliser l’audit (vous pouvez choisir interne ou externe)
+Sur quels critères l’auditeur est choisi ?
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N155" t="inlineStr"/>
       <c r="O155" t="inlineStr"/>
       <c r="P155" t="n">
@@ -5467,7 +6931,17 @@
       <c r="J156" t="inlineStr"/>
       <c r="K156" t="inlineStr"/>
       <c r="L156" t="inlineStr"/>
-      <c r="M156" t="inlineStr"/>
+      <c r="M156" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q3 : PLANIFICATION DE L’AUDIT
+Quelles sont les étapes de l’audit
+Etablir le planning de l’audit (en tenant compte des dates prévues)
+Identifier les acteurs de l’audit et leurs responsabilités (utiliser la matrice RACI)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N156" t="inlineStr"/>
       <c r="O156" t="inlineStr"/>
       <c r="P156" t="n">
@@ -5499,7 +6973,15 @@
       <c r="J157" t="inlineStr"/>
       <c r="K157" t="inlineStr"/>
       <c r="L157" t="inlineStr"/>
-      <c r="M157" t="inlineStr"/>
+      <c r="M157" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q4 : ANALYSE DOCUMENTAIRE
+Quels sont les documents qui pourraient vous aider à préparer cet audit ? (Soyez précis, vous pouvez identifier des documents que DISTRELEC pourrait avoir)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N157" t="inlineStr"/>
       <c r="O157" t="inlineStr"/>
       <c r="P157" t="n">
@@ -5531,7 +7013,16 @@
       <c r="J158" t="inlineStr"/>
       <c r="K158" t="inlineStr"/>
       <c r="L158" t="inlineStr"/>
-      <c r="M158" t="inlineStr"/>
+      <c r="M158" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q5 : REALISATION DE L’AUDIT
+Identifier 3 personnes (fonctions) à auditer
+Elaborer le guide d’entretien pour l’un des audités (préciser lequel)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N158" t="inlineStr"/>
       <c r="O158" t="inlineStr"/>
       <c r="P158" t="n">
@@ -5563,7 +7054,18 @@
       <c r="J159" t="inlineStr"/>
       <c r="K159" t="inlineStr"/>
       <c r="L159" t="inlineStr"/>
-      <c r="M159" t="inlineStr"/>
+      <c r="M159" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q6 : CONCLUSIONS DE L’AUDIT
+Rédiger votre conclusion (à imaginer) présentant : 
+☞ 1 point fort
+☞ 2 points sensibles
+☞ 2 écarts
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N159" t="inlineStr"/>
       <c r="O159" t="inlineStr"/>
       <c r="P159" t="n">
@@ -5595,7 +7097,15 @@
       <c r="J160" t="inlineStr"/>
       <c r="K160" t="inlineStr"/>
       <c r="L160" t="inlineStr"/>
-      <c r="M160" t="inlineStr"/>
+      <c r="M160" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q7 : RECHERCHE DES CAUSES
+Pour chaque écart relevé identifier faite une analyse des causes (en utilisant le diagramme 5M)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N160" t="inlineStr"/>
       <c r="O160" t="inlineStr"/>
       <c r="P160" t="n">
@@ -5627,7 +7137,17 @@
       <c r="J161" t="inlineStr"/>
       <c r="K161" t="inlineStr"/>
       <c r="L161" t="inlineStr"/>
-      <c r="M161" t="inlineStr"/>
+      <c r="M161" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q8 : SOLUTIONS
+Trouver 2 solutions pour chaque écart : 
+☞ Préciser à quelles causes elles correspondent
+☞ Décrire les solutions
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N161" t="inlineStr"/>
       <c r="O161" t="inlineStr"/>
       <c r="P161" t="n">
@@ -5659,7 +7179,17 @@
       <c r="J162" t="inlineStr"/>
       <c r="K162" t="inlineStr"/>
       <c r="L162" t="inlineStr"/>
-      <c r="M162" t="inlineStr"/>
+      <c r="M162" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q1 : ANALYSE DES RISQUES
+Quels sont les risques engendrés par cette situation
+Evaluer ces risques
+Identifier ceux qui sont critiques – et pourquoi (vous pouvez vous servir de la matrice de criticité des risques)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N162" t="inlineStr"/>
       <c r="O162" t="inlineStr"/>
       <c r="P162" t="n">
@@ -5691,7 +7221,17 @@
       <c r="J163" t="inlineStr"/>
       <c r="K163" t="inlineStr"/>
       <c r="L163" t="inlineStr"/>
-      <c r="M163" t="inlineStr"/>
+      <c r="M163" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q2 : DECLENCHEMENT DE L’AUDIT
+Qui mandate l’audit
+Qui va réaliser l’audit (vous pouvez choisir interne ou externe)
+Sur quels critères l’auditeur est choisi ?
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N163" t="inlineStr"/>
       <c r="O163" t="inlineStr"/>
       <c r="P163" t="n">
@@ -5723,7 +7263,17 @@
       <c r="J164" t="inlineStr"/>
       <c r="K164" t="inlineStr"/>
       <c r="L164" t="inlineStr"/>
-      <c r="M164" t="inlineStr"/>
+      <c r="M164" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q3 : PLANIFICATION DE L’AUDIT
+Quelles sont les étapes de l’audit
+Etablir le planning de l’audit (en tenant compte des dates prévues)
+Identifier les acteurs de l’audit et leurs responsabilités (utiliser la matrice RACI)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N164" t="inlineStr"/>
       <c r="O164" t="inlineStr"/>
       <c r="P164" t="n">
@@ -5755,7 +7305,15 @@
       <c r="J165" t="inlineStr"/>
       <c r="K165" t="inlineStr"/>
       <c r="L165" t="inlineStr"/>
-      <c r="M165" t="inlineStr"/>
+      <c r="M165" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q4 : ANALYSE DOCUMENTAIRE
+Quels sont les documents qui pourraient vous aider à préparer cet audit ? (Soyez précis, vous pouvez identifier des documents que DISTRELEC pourrait avoir)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N165" t="inlineStr"/>
       <c r="O165" t="inlineStr"/>
       <c r="P165" t="n">
@@ -5787,7 +7345,16 @@
       <c r="J166" t="inlineStr"/>
       <c r="K166" t="inlineStr"/>
       <c r="L166" t="inlineStr"/>
-      <c r="M166" t="inlineStr"/>
+      <c r="M166" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q5 : REALISATION DE L’AUDIT
+Identifier 3 personnes (fonctions) à auditer
+Elaborer le guide d’entretien pour l’un des audités (préciser lequel)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N166" t="inlineStr"/>
       <c r="O166" t="inlineStr"/>
       <c r="P166" t="n">
@@ -5819,7 +7386,18 @@
       <c r="J167" t="inlineStr"/>
       <c r="K167" t="inlineStr"/>
       <c r="L167" t="inlineStr"/>
-      <c r="M167" t="inlineStr"/>
+      <c r="M167" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q6 : CONCLUSIONS DE L’AUDIT
+Rédiger votre conclusion (à imaginer) présentant : 
+☞ 1 point fort
+☞ 2 points sensibles
+☞ 2 écarts
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N167" t="inlineStr"/>
       <c r="O167" t="inlineStr"/>
       <c r="P167" t="n">
@@ -5851,7 +7429,15 @@
       <c r="J168" t="inlineStr"/>
       <c r="K168" t="inlineStr"/>
       <c r="L168" t="inlineStr"/>
-      <c r="M168" t="inlineStr"/>
+      <c r="M168" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q7 : RECHERCHE DES CAUSES
+Pour chaque écart relevé identifier faite une analyse des causes (en utilisant le diagramme 5M)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N168" t="inlineStr"/>
       <c r="O168" t="inlineStr"/>
       <c r="P168" t="n">
@@ -5883,7 +7469,17 @@
       <c r="J169" t="inlineStr"/>
       <c r="K169" t="inlineStr"/>
       <c r="L169" t="inlineStr"/>
-      <c r="M169" t="inlineStr"/>
+      <c r="M169" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q8 : SOLUTIONS
+Trouver 2 solutions pour chaque écart : 
+☞ Préciser à quelles causes elles correspondent
+☞ Décrire les solutions
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N169" t="inlineStr"/>
       <c r="O169" t="inlineStr"/>
       <c r="P169" t="n">
@@ -5915,7 +7511,17 @@
       <c r="J170" t="inlineStr"/>
       <c r="K170" t="inlineStr"/>
       <c r="L170" t="inlineStr"/>
-      <c r="M170" t="inlineStr"/>
+      <c r="M170" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q1 : ANALYSE DES RISQUES
+Quels sont les risques engendrés par cette situation
+Evaluer ces risques
+Identifier ceux qui sont critiques – et pourquoi (vous pouvez vous servir de la matrice de criticité des risques)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N170" t="inlineStr"/>
       <c r="O170" t="inlineStr"/>
       <c r="P170" t="n">
@@ -5947,7 +7553,17 @@
       <c r="J171" t="inlineStr"/>
       <c r="K171" t="inlineStr"/>
       <c r="L171" t="inlineStr"/>
-      <c r="M171" t="inlineStr"/>
+      <c r="M171" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q2 : DECLENCHEMENT DE L’AUDIT
+Qui mandate l’audit
+Qui va réaliser l’audit (vous pouvez choisir interne ou externe)
+Sur quels critères l’auditeur est choisi ?
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N171" t="inlineStr"/>
       <c r="O171" t="inlineStr"/>
       <c r="P171" t="n">
@@ -5979,7 +7595,17 @@
       <c r="J172" t="inlineStr"/>
       <c r="K172" t="inlineStr"/>
       <c r="L172" t="inlineStr"/>
-      <c r="M172" t="inlineStr"/>
+      <c r="M172" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q3 : PLANIFICATION DE L’AUDIT
+Quelles sont les étapes de l’audit
+Etablir le planning de l’audit (en tenant compte des dates prévues)
+Identifier les acteurs de l’audit et leurs responsabilités (utiliser la matrice RACI)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N172" t="inlineStr"/>
       <c r="O172" t="inlineStr"/>
       <c r="P172" t="n">
@@ -6011,7 +7637,15 @@
       <c r="J173" t="inlineStr"/>
       <c r="K173" t="inlineStr"/>
       <c r="L173" t="inlineStr"/>
-      <c r="M173" t="inlineStr"/>
+      <c r="M173" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q4 : ANALYSE DOCUMENTAIRE
+Quels sont les documents qui pourraient vous aider à préparer cet audit ? (Soyez précis, vous pouvez identifier des documents que DISTRELEC pourrait avoir)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N173" t="inlineStr"/>
       <c r="O173" t="inlineStr"/>
       <c r="P173" t="n">
@@ -6043,7 +7677,16 @@
       <c r="J174" t="inlineStr"/>
       <c r="K174" t="inlineStr"/>
       <c r="L174" t="inlineStr"/>
-      <c r="M174" t="inlineStr"/>
+      <c r="M174" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q5 : REALISATION DE L’AUDIT
+Identifier 3 personnes (fonctions) à auditer
+Elaborer le guide d’entretien pour l’un des audités (préciser lequel)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N174" t="inlineStr"/>
       <c r="O174" t="inlineStr"/>
       <c r="P174" t="n">
@@ -6075,7 +7718,18 @@
       <c r="J175" t="inlineStr"/>
       <c r="K175" t="inlineStr"/>
       <c r="L175" t="inlineStr"/>
-      <c r="M175" t="inlineStr"/>
+      <c r="M175" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q6 : CONCLUSIONS DE L’AUDIT
+Rédiger votre conclusion (à imaginer) présentant : 
+☞ 1 point fort
+☞ 2 points sensibles
+☞ 2 écarts
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N175" t="inlineStr"/>
       <c r="O175" t="inlineStr"/>
       <c r="P175" t="n">
@@ -6107,7 +7761,15 @@
       <c r="J176" t="inlineStr"/>
       <c r="K176" t="inlineStr"/>
       <c r="L176" t="inlineStr"/>
-      <c r="M176" t="inlineStr"/>
+      <c r="M176" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q7 : RECHERCHE DES CAUSES
+Pour chaque écart relevé identifier faite une analyse des causes (en utilisant le diagramme 5M)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N176" t="inlineStr"/>
       <c r="O176" t="inlineStr"/>
       <c r="P176" t="n">
@@ -6139,7 +7801,17 @@
       <c r="J177" t="inlineStr"/>
       <c r="K177" t="inlineStr"/>
       <c r="L177" t="inlineStr"/>
-      <c r="M177" t="inlineStr"/>
+      <c r="M177" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q8 : SOLUTIONS
+Trouver 2 solutions pour chaque écart : 
+☞ Préciser à quelles causes elles correspondent
+☞ Décrire les solutions
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N177" t="inlineStr"/>
       <c r="O177" t="inlineStr"/>
       <c r="P177" t="n">
@@ -6171,7 +7843,17 @@
       <c r="J178" t="inlineStr"/>
       <c r="K178" t="inlineStr"/>
       <c r="L178" t="inlineStr"/>
-      <c r="M178" t="inlineStr"/>
+      <c r="M178" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q1 : ANALYSE DES RISQUES
+Quels sont les risques engendrés par cette situation
+Evaluer ces risques
+Identifier ceux qui sont critiques – et pourquoi (vous pouvez vous servir de la matrice de criticité des risques)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N178" t="inlineStr"/>
       <c r="O178" t="inlineStr"/>
       <c r="P178" t="n">
@@ -6203,7 +7885,17 @@
       <c r="J179" t="inlineStr"/>
       <c r="K179" t="inlineStr"/>
       <c r="L179" t="inlineStr"/>
-      <c r="M179" t="inlineStr"/>
+      <c r="M179" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q2 : DECLENCHEMENT DE L’AUDIT
+Qui mandate l’audit
+Qui va réaliser l’audit (vous pouvez choisir interne ou externe)
+Sur quels critères l’auditeur est choisi ?
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N179" t="inlineStr"/>
       <c r="O179" t="inlineStr"/>
       <c r="P179" t="n">
@@ -6235,7 +7927,17 @@
       <c r="J180" t="inlineStr"/>
       <c r="K180" t="inlineStr"/>
       <c r="L180" t="inlineStr"/>
-      <c r="M180" t="inlineStr"/>
+      <c r="M180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q3 : PLANIFICATION DE L’AUDIT
+Quelles sont les étapes de l’audit
+Etablir le planning de l’audit (en tenant compte des dates prévues)
+Identifier les acteurs de l’audit et leurs responsabilités (utiliser la matrice RACI)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N180" t="inlineStr"/>
       <c r="O180" t="inlineStr"/>
       <c r="P180" t="n">
@@ -6267,7 +7969,15 @@
       <c r="J181" t="inlineStr"/>
       <c r="K181" t="inlineStr"/>
       <c r="L181" t="inlineStr"/>
-      <c r="M181" t="inlineStr"/>
+      <c r="M181" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q4 : ANALYSE DOCUMENTAIRE
+Quels sont les documents qui pourraient vous aider à préparer cet audit ? (Soyez précis, vous pouvez identifier des documents que DISTRELEC pourrait avoir)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N181" t="inlineStr"/>
       <c r="O181" t="inlineStr"/>
       <c r="P181" t="n">
@@ -6299,7 +8009,16 @@
       <c r="J182" t="inlineStr"/>
       <c r="K182" t="inlineStr"/>
       <c r="L182" t="inlineStr"/>
-      <c r="M182" t="inlineStr"/>
+      <c r="M182" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q5 : REALISATION DE L’AUDIT
+Identifier 3 personnes (fonctions) à auditer
+Elaborer le guide d’entretien pour l’un des audités (préciser lequel)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N182" t="inlineStr"/>
       <c r="O182" t="inlineStr"/>
       <c r="P182" t="n">
@@ -6331,7 +8050,18 @@
       <c r="J183" t="inlineStr"/>
       <c r="K183" t="inlineStr"/>
       <c r="L183" t="inlineStr"/>
-      <c r="M183" t="inlineStr"/>
+      <c r="M183" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q6 : CONCLUSIONS DE L’AUDIT
+Rédiger votre conclusion (à imaginer) présentant : 
+☞ 1 point fort
+☞ 2 points sensibles
+☞ 2 écarts
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N183" t="inlineStr"/>
       <c r="O183" t="inlineStr"/>
       <c r="P183" t="n">
@@ -6363,7 +8093,15 @@
       <c r="J184" t="inlineStr"/>
       <c r="K184" t="inlineStr"/>
       <c r="L184" t="inlineStr"/>
-      <c r="M184" t="inlineStr"/>
+      <c r="M184" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q7 : RECHERCHE DES CAUSES
+Pour chaque écart relevé identifier faite une analyse des causes (en utilisant le diagramme 5M)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N184" t="inlineStr"/>
       <c r="O184" t="inlineStr"/>
       <c r="P184" t="n">
@@ -6395,7 +8133,17 @@
       <c r="J185" t="inlineStr"/>
       <c r="K185" t="inlineStr"/>
       <c r="L185" t="inlineStr"/>
-      <c r="M185" t="inlineStr"/>
+      <c r="M185" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q8 : SOLUTIONS
+Trouver 2 solutions pour chaque écart : 
+☞ Préciser à quelles causes elles correspondent
+☞ Décrire les solutions
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N185" t="inlineStr"/>
       <c r="O185" t="inlineStr"/>
       <c r="P185" t="n">
@@ -6427,7 +8175,17 @@
       <c r="J186" t="inlineStr"/>
       <c r="K186" t="inlineStr"/>
       <c r="L186" t="inlineStr"/>
-      <c r="M186" t="inlineStr"/>
+      <c r="M186" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q1 : ANALYSE DES RISQUES
+Quels sont les risques engendrés par cette situation
+Evaluer ces risques
+Identifier ceux qui sont critiques – et pourquoi (vous pouvez vous servir de la matrice de criticité des risques)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N186" t="inlineStr"/>
       <c r="O186" t="inlineStr"/>
       <c r="P186" t="n">
@@ -6459,7 +8217,17 @@
       <c r="J187" t="inlineStr"/>
       <c r="K187" t="inlineStr"/>
       <c r="L187" t="inlineStr"/>
-      <c r="M187" t="inlineStr"/>
+      <c r="M187" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q2 : DECLENCHEMENT DE L’AUDIT
+Qui mandate l’audit
+Qui va réaliser l’audit (vous pouvez choisir interne ou externe)
+Sur quels critères l’auditeur est choisi ?
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N187" t="inlineStr"/>
       <c r="O187" t="inlineStr"/>
       <c r="P187" t="n">
@@ -6491,7 +8259,17 @@
       <c r="J188" t="inlineStr"/>
       <c r="K188" t="inlineStr"/>
       <c r="L188" t="inlineStr"/>
-      <c r="M188" t="inlineStr"/>
+      <c r="M188" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q3 : PLANIFICATION DE L’AUDIT
+Quelles sont les étapes de l’audit
+Etablir le planning de l’audit (en tenant compte des dates prévues)
+Identifier les acteurs de l’audit et leurs responsabilités (utiliser la matrice RACI)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N188" t="inlineStr"/>
       <c r="O188" t="inlineStr"/>
       <c r="P188" t="n">
@@ -6523,7 +8301,15 @@
       <c r="J189" t="inlineStr"/>
       <c r="K189" t="inlineStr"/>
       <c r="L189" t="inlineStr"/>
-      <c r="M189" t="inlineStr"/>
+      <c r="M189" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q4 : ANALYSE DOCUMENTAIRE
+Quels sont les documents qui pourraient vous aider à préparer cet audit ? (Soyez précis, vous pouvez identifier des documents que DISTRELEC pourrait avoir)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N189" t="inlineStr"/>
       <c r="O189" t="inlineStr"/>
       <c r="P189" t="n">
@@ -6555,7 +8341,16 @@
       <c r="J190" t="inlineStr"/>
       <c r="K190" t="inlineStr"/>
       <c r="L190" t="inlineStr"/>
-      <c r="M190" t="inlineStr"/>
+      <c r="M190" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q5 : REALISATION DE L’AUDIT
+Identifier 3 personnes (fonctions) à auditer
+Elaborer le guide d’entretien pour l’un des audités (préciser lequel)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N190" t="inlineStr"/>
       <c r="O190" t="inlineStr"/>
       <c r="P190" t="n">
@@ -6587,7 +8382,18 @@
       <c r="J191" t="inlineStr"/>
       <c r="K191" t="inlineStr"/>
       <c r="L191" t="inlineStr"/>
-      <c r="M191" t="inlineStr"/>
+      <c r="M191" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q6 : CONCLUSIONS DE L’AUDIT
+Rédiger votre conclusion (à imaginer) présentant : 
+☞ 1 point fort
+☞ 2 points sensibles
+☞ 2 écarts
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N191" t="inlineStr"/>
       <c r="O191" t="inlineStr"/>
       <c r="P191" t="n">
@@ -6619,7 +8425,15 @@
       <c r="J192" t="inlineStr"/>
       <c r="K192" t="inlineStr"/>
       <c r="L192" t="inlineStr"/>
-      <c r="M192" t="inlineStr"/>
+      <c r="M192" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q7 : RECHERCHE DES CAUSES
+Pour chaque écart relevé identifier faite une analyse des causes (en utilisant le diagramme 5M)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N192" t="inlineStr"/>
       <c r="O192" t="inlineStr"/>
       <c r="P192" t="n">
@@ -6651,7 +8465,17 @@
       <c r="J193" t="inlineStr"/>
       <c r="K193" t="inlineStr"/>
       <c r="L193" t="inlineStr"/>
-      <c r="M193" t="inlineStr"/>
+      <c r="M193" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q8 : SOLUTIONS
+Trouver 2 solutions pour chaque écart : 
+☞ Préciser à quelles causes elles correspondent
+☞ Décrire les solutions
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N193" t="inlineStr"/>
       <c r="O193" t="inlineStr"/>
       <c r="P193" t="n">
@@ -6683,7 +8507,17 @@
       <c r="J194" t="inlineStr"/>
       <c r="K194" t="inlineStr"/>
       <c r="L194" t="inlineStr"/>
-      <c r="M194" t="inlineStr"/>
+      <c r="M194" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q1 : ANALYSE DES RISQUES
+Quels sont les risques engendrés par cette situation
+Evaluer ces risques
+Identifier ceux qui sont critiques – et pourquoi (vous pouvez vous servir de la matrice de criticité des risques)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N194" t="inlineStr"/>
       <c r="O194" t="inlineStr"/>
       <c r="P194" t="n">
@@ -6715,7 +8549,17 @@
       <c r="J195" t="inlineStr"/>
       <c r="K195" t="inlineStr"/>
       <c r="L195" t="inlineStr"/>
-      <c r="M195" t="inlineStr"/>
+      <c r="M195" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q2 : DECLENCHEMENT DE L’AUDIT
+Qui mandate l’audit
+Qui va réaliser l’audit (vous pouvez choisir interne ou externe)
+Sur quels critères l’auditeur est choisi ?
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N195" t="inlineStr"/>
       <c r="O195" t="inlineStr"/>
       <c r="P195" t="n">
@@ -6747,7 +8591,17 @@
       <c r="J196" t="inlineStr"/>
       <c r="K196" t="inlineStr"/>
       <c r="L196" t="inlineStr"/>
-      <c r="M196" t="inlineStr"/>
+      <c r="M196" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q3 : PLANIFICATION DE L’AUDIT
+Quelles sont les étapes de l’audit
+Etablir le planning de l’audit (en tenant compte des dates prévues)
+Identifier les acteurs de l’audit et leurs responsabilités (utiliser la matrice RACI)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N196" t="inlineStr"/>
       <c r="O196" t="inlineStr"/>
       <c r="P196" t="n">
@@ -6779,7 +8633,15 @@
       <c r="J197" t="inlineStr"/>
       <c r="K197" t="inlineStr"/>
       <c r="L197" t="inlineStr"/>
-      <c r="M197" t="inlineStr"/>
+      <c r="M197" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q4 : ANALYSE DOCUMENTAIRE
+Quels sont les documents qui pourraient vous aider à préparer cet audit ? (Soyez précis, vous pouvez identifier des documents que DISTRELEC pourrait avoir)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N197" t="inlineStr"/>
       <c r="O197" t="inlineStr"/>
       <c r="P197" t="n">
@@ -6811,7 +8673,16 @@
       <c r="J198" t="inlineStr"/>
       <c r="K198" t="inlineStr"/>
       <c r="L198" t="inlineStr"/>
-      <c r="M198" t="inlineStr"/>
+      <c r="M198" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q5 : REALISATION DE L’AUDIT
+Identifier 3 personnes (fonctions) à auditer
+Elaborer le guide d’entretien pour l’un des audités (préciser lequel)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N198" t="inlineStr"/>
       <c r="O198" t="inlineStr"/>
       <c r="P198" t="n">
@@ -6843,7 +8714,18 @@
       <c r="J199" t="inlineStr"/>
       <c r="K199" t="inlineStr"/>
       <c r="L199" t="inlineStr"/>
-      <c r="M199" t="inlineStr"/>
+      <c r="M199" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q6 : CONCLUSIONS DE L’AUDIT
+Rédiger votre conclusion (à imaginer) présentant : 
+☞ 1 point fort
+☞ 2 points sensibles
+☞ 2 écarts
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N199" t="inlineStr"/>
       <c r="O199" t="inlineStr"/>
       <c r="P199" t="n">
@@ -6875,7 +8757,15 @@
       <c r="J200" t="inlineStr"/>
       <c r="K200" t="inlineStr"/>
       <c r="L200" t="inlineStr"/>
-      <c r="M200" t="inlineStr"/>
+      <c r="M200" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q7 : RECHERCHE DES CAUSES
+Pour chaque écart relevé identifier faite une analyse des causes (en utilisant le diagramme 5M)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N200" t="inlineStr"/>
       <c r="O200" t="inlineStr"/>
       <c r="P200" t="n">
@@ -6907,7 +8797,17 @@
       <c r="J201" t="inlineStr"/>
       <c r="K201" t="inlineStr"/>
       <c r="L201" t="inlineStr"/>
-      <c r="M201" t="inlineStr"/>
+      <c r="M201" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q8 : SOLUTIONS
+Trouver 2 solutions pour chaque écart : 
+☞ Préciser à quelles causes elles correspondent
+☞ Décrire les solutions
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N201" t="inlineStr"/>
       <c r="O201" t="inlineStr"/>
       <c r="P201" t="n">
@@ -6939,7 +8839,17 @@
       <c r="J202" t="inlineStr"/>
       <c r="K202" t="inlineStr"/>
       <c r="L202" t="inlineStr"/>
-      <c r="M202" t="inlineStr"/>
+      <c r="M202" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q1 : ANALYSE DES RISQUES
+Quels sont les risques engendrés par cette situation
+Evaluer ces risques
+Identifier ceux qui sont critiques – et pourquoi (vous pouvez vous servir de la matrice de criticité des risques)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N202" t="inlineStr"/>
       <c r="O202" t="inlineStr"/>
       <c r="P202" t="n">
@@ -6971,7 +8881,17 @@
       <c r="J203" t="inlineStr"/>
       <c r="K203" t="inlineStr"/>
       <c r="L203" t="inlineStr"/>
-      <c r="M203" t="inlineStr"/>
+      <c r="M203" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q2 : DECLENCHEMENT DE L’AUDIT
+Qui mandate l’audit
+Qui va réaliser l’audit (vous pouvez choisir interne ou externe)
+Sur quels critères l’auditeur est choisi ?
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N203" t="inlineStr"/>
       <c r="O203" t="inlineStr"/>
       <c r="P203" t="n">
@@ -7003,7 +8923,17 @@
       <c r="J204" t="inlineStr"/>
       <c r="K204" t="inlineStr"/>
       <c r="L204" t="inlineStr"/>
-      <c r="M204" t="inlineStr"/>
+      <c r="M204" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q3 : PLANIFICATION DE L’AUDIT
+Quelles sont les étapes de l’audit
+Etablir le planning de l’audit (en tenant compte des dates prévues)
+Identifier les acteurs de l’audit et leurs responsabilités (utiliser la matrice RACI)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N204" t="inlineStr"/>
       <c r="O204" t="inlineStr"/>
       <c r="P204" t="n">
@@ -7035,7 +8965,15 @@
       <c r="J205" t="inlineStr"/>
       <c r="K205" t="inlineStr"/>
       <c r="L205" t="inlineStr"/>
-      <c r="M205" t="inlineStr"/>
+      <c r="M205" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q4 : ANALYSE DOCUMENTAIRE
+Quels sont les documents qui pourraient vous aider à préparer cet audit ? (Soyez précis, vous pouvez identifier des documents que DISTRELEC pourrait avoir)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N205" t="inlineStr"/>
       <c r="O205" t="inlineStr"/>
       <c r="P205" t="n">
@@ -7067,7 +9005,16 @@
       <c r="J206" t="inlineStr"/>
       <c r="K206" t="inlineStr"/>
       <c r="L206" t="inlineStr"/>
-      <c r="M206" t="inlineStr"/>
+      <c r="M206" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q5 : REALISATION DE L’AUDIT
+Identifier 3 personnes (fonctions) à auditer
+Elaborer le guide d’entretien pour l’un des audités (préciser lequel)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N206" t="inlineStr"/>
       <c r="O206" t="inlineStr"/>
       <c r="P206" t="n">
@@ -7099,7 +9046,18 @@
       <c r="J207" t="inlineStr"/>
       <c r="K207" t="inlineStr"/>
       <c r="L207" t="inlineStr"/>
-      <c r="M207" t="inlineStr"/>
+      <c r="M207" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q6 : CONCLUSIONS DE L’AUDIT
+Rédiger votre conclusion (à imaginer) présentant : 
+☞ 1 point fort
+☞ 2 points sensibles
+☞ 2 écarts
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N207" t="inlineStr"/>
       <c r="O207" t="inlineStr"/>
       <c r="P207" t="n">
@@ -7131,7 +9089,15 @@
       <c r="J208" t="inlineStr"/>
       <c r="K208" t="inlineStr"/>
       <c r="L208" t="inlineStr"/>
-      <c r="M208" t="inlineStr"/>
+      <c r="M208" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q7 : RECHERCHE DES CAUSES
+Pour chaque écart relevé identifier faite une analyse des causes (en utilisant le diagramme 5M)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N208" t="inlineStr"/>
       <c r="O208" t="inlineStr"/>
       <c r="P208" t="n">
@@ -7163,7 +9129,17 @@
       <c r="J209" t="inlineStr"/>
       <c r="K209" t="inlineStr"/>
       <c r="L209" t="inlineStr"/>
-      <c r="M209" t="inlineStr"/>
+      <c r="M209" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q8 : SOLUTIONS
+Trouver 2 solutions pour chaque écart : 
+☞ Préciser à quelles causes elles correspondent
+☞ Décrire les solutions
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N209" t="inlineStr"/>
       <c r="O209" t="inlineStr"/>
       <c r="P209" t="n">
@@ -7195,7 +9171,17 @@
       <c r="J210" t="inlineStr"/>
       <c r="K210" t="inlineStr"/>
       <c r="L210" t="inlineStr"/>
-      <c r="M210" t="inlineStr"/>
+      <c r="M210" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q1 : ANALYSE DES RISQUES
+Quels sont les risques engendrés par cette situation
+Evaluer ces risques
+Identifier ceux qui sont critiques – et pourquoi (vous pouvez vous servir de la matrice de criticité des risques)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N210" t="inlineStr"/>
       <c r="O210" t="inlineStr"/>
       <c r="P210" t="n">
@@ -7227,7 +9213,17 @@
       <c r="J211" t="inlineStr"/>
       <c r="K211" t="inlineStr"/>
       <c r="L211" t="inlineStr"/>
-      <c r="M211" t="inlineStr"/>
+      <c r="M211" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q2 : DECLENCHEMENT DE L’AUDIT
+Qui mandate l’audit
+Qui va réaliser l’audit (vous pouvez choisir interne ou externe)
+Sur quels critères l’auditeur est choisi ?
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N211" t="inlineStr"/>
       <c r="O211" t="inlineStr"/>
       <c r="P211" t="n">
@@ -7259,7 +9255,17 @@
       <c r="J212" t="inlineStr"/>
       <c r="K212" t="inlineStr"/>
       <c r="L212" t="inlineStr"/>
-      <c r="M212" t="inlineStr"/>
+      <c r="M212" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q3 : PLANIFICATION DE L’AUDIT
+Quelles sont les étapes de l’audit
+Etablir le planning de l’audit (en tenant compte des dates prévues)
+Identifier les acteurs de l’audit et leurs responsabilités (utiliser la matrice RACI)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N212" t="inlineStr"/>
       <c r="O212" t="inlineStr"/>
       <c r="P212" t="n">
@@ -7291,7 +9297,15 @@
       <c r="J213" t="inlineStr"/>
       <c r="K213" t="inlineStr"/>
       <c r="L213" t="inlineStr"/>
-      <c r="M213" t="inlineStr"/>
+      <c r="M213" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q4 : ANALYSE DOCUMENTAIRE
+Quels sont les documents qui pourraient vous aider à préparer cet audit ? (Soyez précis, vous pouvez identifier des documents que DISTRELEC pourrait avoir)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N213" t="inlineStr"/>
       <c r="O213" t="inlineStr"/>
       <c r="P213" t="n">
@@ -7323,7 +9337,16 @@
       <c r="J214" t="inlineStr"/>
       <c r="K214" t="inlineStr"/>
       <c r="L214" t="inlineStr"/>
-      <c r="M214" t="inlineStr"/>
+      <c r="M214" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q5 : REALISATION DE L’AUDIT
+Identifier 3 personnes (fonctions) à auditer
+Elaborer le guide d’entretien pour l’un des audités (préciser lequel)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N214" t="inlineStr"/>
       <c r="O214" t="inlineStr"/>
       <c r="P214" t="n">
@@ -7355,7 +9378,18 @@
       <c r="J215" t="inlineStr"/>
       <c r="K215" t="inlineStr"/>
       <c r="L215" t="inlineStr"/>
-      <c r="M215" t="inlineStr"/>
+      <c r="M215" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q6 : CONCLUSIONS DE L’AUDIT
+Rédiger votre conclusion (à imaginer) présentant : 
+☞ 1 point fort
+☞ 2 points sensibles
+☞ 2 écarts
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N215" t="inlineStr"/>
       <c r="O215" t="inlineStr"/>
       <c r="P215" t="n">
@@ -7387,7 +9421,15 @@
       <c r="J216" t="inlineStr"/>
       <c r="K216" t="inlineStr"/>
       <c r="L216" t="inlineStr"/>
-      <c r="M216" t="inlineStr"/>
+      <c r="M216" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q7 : RECHERCHE DES CAUSES
+Pour chaque écart relevé identifier faite une analyse des causes (en utilisant le diagramme 5M)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N216" t="inlineStr"/>
       <c r="O216" t="inlineStr"/>
       <c r="P216" t="n">
@@ -7419,7 +9461,17 @@
       <c r="J217" t="inlineStr"/>
       <c r="K217" t="inlineStr"/>
       <c r="L217" t="inlineStr"/>
-      <c r="M217" t="inlineStr"/>
+      <c r="M217" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q8 : SOLUTIONS
+Trouver 2 solutions pour chaque écart : 
+☞ Préciser à quelles causes elles correspondent
+☞ Décrire les solutions
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N217" t="inlineStr"/>
       <c r="O217" t="inlineStr"/>
       <c r="P217" t="n">
@@ -7451,7 +9503,17 @@
       <c r="J218" t="inlineStr"/>
       <c r="K218" t="inlineStr"/>
       <c r="L218" t="inlineStr"/>
-      <c r="M218" t="inlineStr"/>
+      <c r="M218" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q1 : ANALYSE DES RISQUES
+Quels sont les risques engendrés par cette situation
+Evaluer ces risques
+Identifier ceux qui sont critiques – et pourquoi (vous pouvez vous servir de la matrice de criticité des risques)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N218" t="inlineStr"/>
       <c r="O218" t="inlineStr"/>
       <c r="P218" t="n">
@@ -7483,7 +9545,17 @@
       <c r="J219" t="inlineStr"/>
       <c r="K219" t="inlineStr"/>
       <c r="L219" t="inlineStr"/>
-      <c r="M219" t="inlineStr"/>
+      <c r="M219" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q2 : DECLENCHEMENT DE L’AUDIT
+Qui mandate l’audit
+Qui va réaliser l’audit (vous pouvez choisir interne ou externe)
+Sur quels critères l’auditeur est choisi ?
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N219" t="inlineStr"/>
       <c r="O219" t="inlineStr"/>
       <c r="P219" t="n">
@@ -7515,7 +9587,17 @@
       <c r="J220" t="inlineStr"/>
       <c r="K220" t="inlineStr"/>
       <c r="L220" t="inlineStr"/>
-      <c r="M220" t="inlineStr"/>
+      <c r="M220" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q3 : PLANIFICATION DE L’AUDIT
+Quelles sont les étapes de l’audit
+Etablir le planning de l’audit (en tenant compte des dates prévues)
+Identifier les acteurs de l’audit et leurs responsabilités (utiliser la matrice RACI)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N220" t="inlineStr"/>
       <c r="O220" t="inlineStr"/>
       <c r="P220" t="n">
@@ -7547,7 +9629,15 @@
       <c r="J221" t="inlineStr"/>
       <c r="K221" t="inlineStr"/>
       <c r="L221" t="inlineStr"/>
-      <c r="M221" t="inlineStr"/>
+      <c r="M221" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q4 : ANALYSE DOCUMENTAIRE
+Quels sont les documents qui pourraient vous aider à préparer cet audit ? (Soyez précis, vous pouvez identifier des documents que DISTRELEC pourrait avoir)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N221" t="inlineStr"/>
       <c r="O221" t="inlineStr"/>
       <c r="P221" t="n">
@@ -7579,7 +9669,16 @@
       <c r="J222" t="inlineStr"/>
       <c r="K222" t="inlineStr"/>
       <c r="L222" t="inlineStr"/>
-      <c r="M222" t="inlineStr"/>
+      <c r="M222" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q5 : REALISATION DE L’AUDIT
+Identifier 3 personnes (fonctions) à auditer
+Elaborer le guide d’entretien pour l’un des audités (préciser lequel)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N222" t="inlineStr"/>
       <c r="O222" t="inlineStr"/>
       <c r="P222" t="n">
@@ -7611,7 +9710,18 @@
       <c r="J223" t="inlineStr"/>
       <c r="K223" t="inlineStr"/>
       <c r="L223" t="inlineStr"/>
-      <c r="M223" t="inlineStr"/>
+      <c r="M223" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q6 : CONCLUSIONS DE L’AUDIT
+Rédiger votre conclusion (à imaginer) présentant : 
+☞ 1 point fort
+☞ 2 points sensibles
+☞ 2 écarts
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N223" t="inlineStr"/>
       <c r="O223" t="inlineStr"/>
       <c r="P223" t="n">
@@ -7643,7 +9753,15 @@
       <c r="J224" t="inlineStr"/>
       <c r="K224" t="inlineStr"/>
       <c r="L224" t="inlineStr"/>
-      <c r="M224" t="inlineStr"/>
+      <c r="M224" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q7 : RECHERCHE DES CAUSES
+Pour chaque écart relevé identifier faite une analyse des causes (en utilisant le diagramme 5M)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N224" t="inlineStr"/>
       <c r="O224" t="inlineStr"/>
       <c r="P224" t="n">
@@ -7675,7 +9793,17 @@
       <c r="J225" t="inlineStr"/>
       <c r="K225" t="inlineStr"/>
       <c r="L225" t="inlineStr"/>
-      <c r="M225" t="inlineStr"/>
+      <c r="M225" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q8 : SOLUTIONS
+Trouver 2 solutions pour chaque écart : 
+☞ Préciser à quelles causes elles correspondent
+☞ Décrire les solutions
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N225" t="inlineStr"/>
       <c r="O225" t="inlineStr"/>
       <c r="P225" t="n">
@@ -7707,7 +9835,17 @@
       <c r="J226" t="inlineStr"/>
       <c r="K226" t="inlineStr"/>
       <c r="L226" t="inlineStr"/>
-      <c r="M226" t="inlineStr"/>
+      <c r="M226" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q1 : ANALYSE DES RISQUES
+Quels sont les risques engendrés par cette situation
+Evaluer ces risques
+Identifier ceux qui sont critiques – et pourquoi (vous pouvez vous servir de la matrice de criticité des risques)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N226" t="inlineStr"/>
       <c r="O226" t="inlineStr"/>
       <c r="P226" t="n">
@@ -7739,7 +9877,17 @@
       <c r="J227" t="inlineStr"/>
       <c r="K227" t="inlineStr"/>
       <c r="L227" t="inlineStr"/>
-      <c r="M227" t="inlineStr"/>
+      <c r="M227" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q2 : DECLENCHEMENT DE L’AUDIT
+Qui mandate l’audit
+Qui va réaliser l’audit (vous pouvez choisir interne ou externe)
+Sur quels critères l’auditeur est choisi ?
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N227" t="inlineStr"/>
       <c r="O227" t="inlineStr"/>
       <c r="P227" t="n">
@@ -7771,7 +9919,17 @@
       <c r="J228" t="inlineStr"/>
       <c r="K228" t="inlineStr"/>
       <c r="L228" t="inlineStr"/>
-      <c r="M228" t="inlineStr"/>
+      <c r="M228" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q3 : PLANIFICATION DE L’AUDIT
+Quelles sont les étapes de l’audit
+Etablir le planning de l’audit (en tenant compte des dates prévues)
+Identifier les acteurs de l’audit et leurs responsabilités (utiliser la matrice RACI)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N228" t="inlineStr"/>
       <c r="O228" t="inlineStr"/>
       <c r="P228" t="n">
@@ -7803,7 +9961,15 @@
       <c r="J229" t="inlineStr"/>
       <c r="K229" t="inlineStr"/>
       <c r="L229" t="inlineStr"/>
-      <c r="M229" t="inlineStr"/>
+      <c r="M229" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q4 : ANALYSE DOCUMENTAIRE
+Quels sont les documents qui pourraient vous aider à préparer cet audit ? (Soyez précis, vous pouvez identifier des documents que DISTRELEC pourrait avoir)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N229" t="inlineStr"/>
       <c r="O229" t="inlineStr"/>
       <c r="P229" t="n">
@@ -7835,7 +10001,16 @@
       <c r="J230" t="inlineStr"/>
       <c r="K230" t="inlineStr"/>
       <c r="L230" t="inlineStr"/>
-      <c r="M230" t="inlineStr"/>
+      <c r="M230" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q5 : REALISATION DE L’AUDIT
+Identifier 3 personnes (fonctions) à auditer
+Elaborer le guide d’entretien pour l’un des audités (préciser lequel)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N230" t="inlineStr"/>
       <c r="O230" t="inlineStr"/>
       <c r="P230" t="n">
@@ -7867,7 +10042,18 @@
       <c r="J231" t="inlineStr"/>
       <c r="K231" t="inlineStr"/>
       <c r="L231" t="inlineStr"/>
-      <c r="M231" t="inlineStr"/>
+      <c r="M231" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q6 : CONCLUSIONS DE L’AUDIT
+Rédiger votre conclusion (à imaginer) présentant : 
+☞ 1 point fort
+☞ 2 points sensibles
+☞ 2 écarts
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N231" t="inlineStr"/>
       <c r="O231" t="inlineStr"/>
       <c r="P231" t="n">
@@ -7899,7 +10085,15 @@
       <c r="J232" t="inlineStr"/>
       <c r="K232" t="inlineStr"/>
       <c r="L232" t="inlineStr"/>
-      <c r="M232" t="inlineStr"/>
+      <c r="M232" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q7 : RECHERCHE DES CAUSES
+Pour chaque écart relevé identifier faite une analyse des causes (en utilisant le diagramme 5M)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N232" t="inlineStr"/>
       <c r="O232" t="inlineStr"/>
       <c r="P232" t="n">
@@ -7931,7 +10125,17 @@
       <c r="J233" t="inlineStr"/>
       <c r="K233" t="inlineStr"/>
       <c r="L233" t="inlineStr"/>
-      <c r="M233" t="inlineStr"/>
+      <c r="M233" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q8 : SOLUTIONS
+Trouver 2 solutions pour chaque écart : 
+☞ Préciser à quelles causes elles correspondent
+☞ Décrire les solutions
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N233" t="inlineStr"/>
       <c r="O233" t="inlineStr"/>
       <c r="P233" t="n">
@@ -7963,7 +10167,17 @@
       <c r="J234" t="inlineStr"/>
       <c r="K234" t="inlineStr"/>
       <c r="L234" t="inlineStr"/>
-      <c r="M234" t="inlineStr"/>
+      <c r="M234" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q1 : ANALYSE DES RISQUES
+Quels sont les risques engendrés par cette situation
+Evaluer ces risques
+Identifier ceux qui sont critiques – et pourquoi (vous pouvez vous servir de la matrice de criticité des risques)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N234" t="inlineStr"/>
       <c r="O234" t="inlineStr"/>
       <c r="P234" t="n">
@@ -7995,7 +10209,17 @@
       <c r="J235" t="inlineStr"/>
       <c r="K235" t="inlineStr"/>
       <c r="L235" t="inlineStr"/>
-      <c r="M235" t="inlineStr"/>
+      <c r="M235" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q2 : DECLENCHEMENT DE L’AUDIT
+Qui mandate l’audit
+Qui va réaliser l’audit (vous pouvez choisir interne ou externe)
+Sur quels critères l’auditeur est choisi ?
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N235" t="inlineStr"/>
       <c r="O235" t="inlineStr"/>
       <c r="P235" t="n">
@@ -8027,7 +10251,17 @@
       <c r="J236" t="inlineStr"/>
       <c r="K236" t="inlineStr"/>
       <c r="L236" t="inlineStr"/>
-      <c r="M236" t="inlineStr"/>
+      <c r="M236" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q3 : PLANIFICATION DE L’AUDIT
+Quelles sont les étapes de l’audit
+Etablir le planning de l’audit (en tenant compte des dates prévues)
+Identifier les acteurs de l’audit et leurs responsabilités (utiliser la matrice RACI)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N236" t="inlineStr"/>
       <c r="O236" t="inlineStr"/>
       <c r="P236" t="n">
@@ -8059,7 +10293,15 @@
       <c r="J237" t="inlineStr"/>
       <c r="K237" t="inlineStr"/>
       <c r="L237" t="inlineStr"/>
-      <c r="M237" t="inlineStr"/>
+      <c r="M237" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q4 : ANALYSE DOCUMENTAIRE
+Quels sont les documents qui pourraient vous aider à préparer cet audit ? (Soyez précis, vous pouvez identifier des documents que DISTRELEC pourrait avoir)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N237" t="inlineStr"/>
       <c r="O237" t="inlineStr"/>
       <c r="P237" t="n">
@@ -8091,7 +10333,16 @@
       <c r="J238" t="inlineStr"/>
       <c r="K238" t="inlineStr"/>
       <c r="L238" t="inlineStr"/>
-      <c r="M238" t="inlineStr"/>
+      <c r="M238" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q5 : REALISATION DE L’AUDIT
+Identifier 3 personnes (fonctions) à auditer
+Elaborer le guide d’entretien pour l’un des audités (préciser lequel)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N238" t="inlineStr"/>
       <c r="O238" t="inlineStr"/>
       <c r="P238" t="n">
@@ -8123,7 +10374,18 @@
       <c r="J239" t="inlineStr"/>
       <c r="K239" t="inlineStr"/>
       <c r="L239" t="inlineStr"/>
-      <c r="M239" t="inlineStr"/>
+      <c r="M239" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q6 : CONCLUSIONS DE L’AUDIT
+Rédiger votre conclusion (à imaginer) présentant : 
+☞ 1 point fort
+☞ 2 points sensibles
+☞ 2 écarts
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N239" t="inlineStr"/>
       <c r="O239" t="inlineStr"/>
       <c r="P239" t="n">
@@ -8155,7 +10417,15 @@
       <c r="J240" t="inlineStr"/>
       <c r="K240" t="inlineStr"/>
       <c r="L240" t="inlineStr"/>
-      <c r="M240" t="inlineStr"/>
+      <c r="M240" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q7 : RECHERCHE DES CAUSES
+Pour chaque écart relevé identifier faite une analyse des causes (en utilisant le diagramme 5M)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N240" t="inlineStr"/>
       <c r="O240" t="inlineStr"/>
       <c r="P240" t="n">
@@ -8187,7 +10457,17 @@
       <c r="J241" t="inlineStr"/>
       <c r="K241" t="inlineStr"/>
       <c r="L241" t="inlineStr"/>
-      <c r="M241" t="inlineStr"/>
+      <c r="M241" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q8 : SOLUTIONS
+Trouver 2 solutions pour chaque écart : 
+☞ Préciser à quelles causes elles correspondent
+☞ Décrire les solutions
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N241" t="inlineStr"/>
       <c r="O241" t="inlineStr"/>
       <c r="P241" t="n">
@@ -8219,7 +10499,17 @@
       <c r="J242" t="inlineStr"/>
       <c r="K242" t="inlineStr"/>
       <c r="L242" t="inlineStr"/>
-      <c r="M242" t="inlineStr"/>
+      <c r="M242" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q1 : ANALYSE DES RISQUES
+Quels sont les risques engendrés par cette situation
+Evaluer ces risques
+Identifier ceux qui sont critiques – et pourquoi (vous pouvez vous servir de la matrice de criticité des risques)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N242" t="inlineStr"/>
       <c r="O242" t="inlineStr"/>
       <c r="P242" t="n">
@@ -8251,7 +10541,17 @@
       <c r="J243" t="inlineStr"/>
       <c r="K243" t="inlineStr"/>
       <c r="L243" t="inlineStr"/>
-      <c r="M243" t="inlineStr"/>
+      <c r="M243" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q2 : DECLENCHEMENT DE L’AUDIT
+Qui mandate l’audit
+Qui va réaliser l’audit (vous pouvez choisir interne ou externe)
+Sur quels critères l’auditeur est choisi ?
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N243" t="inlineStr"/>
       <c r="O243" t="inlineStr"/>
       <c r="P243" t="n">
@@ -8283,7 +10583,17 @@
       <c r="J244" t="inlineStr"/>
       <c r="K244" t="inlineStr"/>
       <c r="L244" t="inlineStr"/>
-      <c r="M244" t="inlineStr"/>
+      <c r="M244" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q3 : PLANIFICATION DE L’AUDIT
+Quelles sont les étapes de l’audit
+Etablir le planning de l’audit (en tenant compte des dates prévues)
+Identifier les acteurs de l’audit et leurs responsabilités (utiliser la matrice RACI)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N244" t="inlineStr"/>
       <c r="O244" t="inlineStr"/>
       <c r="P244" t="n">
@@ -8315,7 +10625,15 @@
       <c r="J245" t="inlineStr"/>
       <c r="K245" t="inlineStr"/>
       <c r="L245" t="inlineStr"/>
-      <c r="M245" t="inlineStr"/>
+      <c r="M245" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q4 : ANALYSE DOCUMENTAIRE
+Quels sont les documents qui pourraient vous aider à préparer cet audit ? (Soyez précis, vous pouvez identifier des documents que DISTRELEC pourrait avoir)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N245" t="inlineStr"/>
       <c r="O245" t="inlineStr"/>
       <c r="P245" t="n">
@@ -8347,7 +10665,16 @@
       <c r="J246" t="inlineStr"/>
       <c r="K246" t="inlineStr"/>
       <c r="L246" t="inlineStr"/>
-      <c r="M246" t="inlineStr"/>
+      <c r="M246" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q5 : REALISATION DE L’AUDIT
+Identifier 3 personnes (fonctions) à auditer
+Elaborer le guide d’entretien pour l’un des audités (préciser lequel)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N246" t="inlineStr"/>
       <c r="O246" t="inlineStr"/>
       <c r="P246" t="n">
@@ -8379,7 +10706,18 @@
       <c r="J247" t="inlineStr"/>
       <c r="K247" t="inlineStr"/>
       <c r="L247" t="inlineStr"/>
-      <c r="M247" t="inlineStr"/>
+      <c r="M247" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q6 : CONCLUSIONS DE L’AUDIT
+Rédiger votre conclusion (à imaginer) présentant : 
+☞ 1 point fort
+☞ 2 points sensibles
+☞ 2 écarts
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N247" t="inlineStr"/>
       <c r="O247" t="inlineStr"/>
       <c r="P247" t="n">
@@ -8411,7 +10749,15 @@
       <c r="J248" t="inlineStr"/>
       <c r="K248" t="inlineStr"/>
       <c r="L248" t="inlineStr"/>
-      <c r="M248" t="inlineStr"/>
+      <c r="M248" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q7 : RECHERCHE DES CAUSES
+Pour chaque écart relevé identifier faite une analyse des causes (en utilisant le diagramme 5M)
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N248" t="inlineStr"/>
       <c r="O248" t="inlineStr"/>
       <c r="P248" t="n">
@@ -8443,7 +10789,17 @@
       <c r="J249" t="inlineStr"/>
       <c r="K249" t="inlineStr"/>
       <c r="L249" t="inlineStr"/>
-      <c r="M249" t="inlineStr"/>
+      <c r="M249" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Q8 : SOLUTIONS
+Trouver 2 solutions pour chaque écart : 
+☞ Préciser à quelles causes elles correspondent
+☞ Décrire les solutions
+Votre réponse : 
+</t>
+        </is>
+      </c>
       <c r="N249" t="inlineStr"/>
       <c r="O249" t="inlineStr"/>
       <c r="P249" t="n">

</xml_diff>